<commit_message>
Created function to control ploting
</commit_message>
<xml_diff>
--- a/SCLASurvey.xlsx
+++ b/SCLASurvey.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="68">
   <si>
     <t>LibraryName</t>
   </si>
@@ -209,10 +209,25 @@
     <t>LibrarianIIISalHigh</t>
   </si>
   <si>
-    <t>LibrarianIIIWageLow</t>
-  </si>
-  <si>
-    <t>LibrarianIIIWageHigh</t>
+    <t>WeeklyHours</t>
+  </si>
+  <si>
+    <t>LibraryTraineeWageLow</t>
+  </si>
+  <si>
+    <t>LibraryTraineeWageHigh</t>
+  </si>
+  <si>
+    <t>LibraryTraineeSalLow</t>
+  </si>
+  <si>
+    <t>LibraryTraineeSalHigh</t>
+  </si>
+  <si>
+    <t>LibrarianISalLow</t>
+  </si>
+  <si>
+    <t>LibrarianISalHigh</t>
   </si>
 </sst>
 </file>
@@ -530,18 +545,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G57"/>
+  <dimension ref="A1:L57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="E60" sqref="E60"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="H58" sqref="H58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="23.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="0" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="21.1796875" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="0" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="14.54296875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -552,19 +572,34 @@
         <v>58</v>
       </c>
       <c r="D1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H1" t="s">
+        <v>66</v>
+      </c>
+      <c r="I1" t="s">
+        <v>67</v>
+      </c>
+      <c r="J1" t="s">
         <v>59</v>
       </c>
-      <c r="E1" t="s">
+      <c r="K1" t="s">
         <v>60</v>
       </c>
-      <c r="F1" t="s">
+      <c r="L1" t="s">
         <v>61</v>
       </c>
-      <c r="G1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -574,8 +609,14 @@
       <c r="C2">
         <v>40</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="D2">
+        <v>17.5</v>
+      </c>
+      <c r="L2">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -586,13 +627,25 @@
         <v>100</v>
       </c>
       <c r="D3">
+        <v>21.73</v>
+      </c>
+      <c r="E3">
+        <v>22.64</v>
+      </c>
+      <c r="H3">
+        <v>51217</v>
+      </c>
+      <c r="I3">
+        <v>76549</v>
+      </c>
+      <c r="J3">
         <v>60190</v>
       </c>
-      <c r="E3">
+      <c r="K3">
         <v>85713</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -602,36 +655,51 @@
       <c r="C4">
         <v>135</v>
       </c>
-      <c r="D4">
+      <c r="H4">
+        <v>44823</v>
+      </c>
+      <c r="J4">
         <v>48000</v>
       </c>
-      <c r="E4">
+      <c r="K4">
         <v>49000</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="L4">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="B5">
         <v>510</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="L5">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="B6">
         <v>34000</v>
       </c>
-      <c r="D6">
+      <c r="H6">
+        <v>58269</v>
+      </c>
+      <c r="I6">
+        <v>83604</v>
+      </c>
+      <c r="J6">
         <v>68910</v>
       </c>
-      <c r="E6">
+      <c r="K6">
         <v>109445</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -641,14 +709,23 @@
       <c r="C7">
         <v>120</v>
       </c>
-      <c r="D7">
+      <c r="H7">
+        <v>44736</v>
+      </c>
+      <c r="I7">
+        <v>53927</v>
+      </c>
+      <c r="J7">
         <v>64875</v>
       </c>
-      <c r="E7">
+      <c r="K7">
         <v>82859</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="L7">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -658,14 +735,20 @@
       <c r="C8">
         <v>195</v>
       </c>
-      <c r="D8">
+      <c r="H8">
+        <v>53004</v>
+      </c>
+      <c r="J8">
         <v>71525</v>
       </c>
-      <c r="E8">
+      <c r="K8">
         <v>72525</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="L8">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -675,13 +758,19 @@
       <c r="C9">
         <v>35</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H9">
+        <v>42000</v>
+      </c>
+      <c r="L9">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -692,13 +781,34 @@
         <v>100</v>
       </c>
       <c r="D11">
+        <v>16.47</v>
+      </c>
+      <c r="E11">
+        <v>18</v>
+      </c>
+      <c r="F11">
+        <v>36293</v>
+      </c>
+      <c r="G11">
+        <v>57230</v>
+      </c>
+      <c r="H11">
+        <v>45146</v>
+      </c>
+      <c r="I11">
+        <v>71191</v>
+      </c>
+      <c r="J11">
         <v>47889</v>
       </c>
-      <c r="E11">
+      <c r="K11">
         <v>75516</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="L11">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -709,13 +819,28 @@
         <v>122</v>
       </c>
       <c r="D12">
+        <v>23.88</v>
+      </c>
+      <c r="E12">
+        <v>25</v>
+      </c>
+      <c r="H12">
+        <v>45000</v>
+      </c>
+      <c r="I12">
+        <v>47500</v>
+      </c>
+      <c r="J12">
         <v>57200</v>
       </c>
-      <c r="E12">
+      <c r="K12">
         <v>62700</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="L12">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -725,11 +850,11 @@
       <c r="C13">
         <v>65</v>
       </c>
-      <c r="F13">
-        <v>24.3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="L13">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -737,21 +862,39 @@
         <v>160</v>
       </c>
       <c r="D14">
+        <v>19.8</v>
+      </c>
+      <c r="E14">
+        <v>21.8</v>
+      </c>
+      <c r="H14">
+        <v>50128</v>
+      </c>
+      <c r="I14">
+        <v>72462</v>
+      </c>
+      <c r="J14">
         <v>55328</v>
       </c>
-      <c r="E14">
+      <c r="K14">
         <v>80002</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="L14">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>14</v>
       </c>
       <c r="C15">
         <v>250</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="L15">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>56</v>
       </c>
@@ -761,14 +904,23 @@
       <c r="C16">
         <v>250</v>
       </c>
-      <c r="D16">
+      <c r="H16">
+        <v>58614</v>
+      </c>
+      <c r="I16">
+        <v>73055</v>
+      </c>
+      <c r="J16">
         <v>71359</v>
       </c>
-      <c r="E16">
+      <c r="K16">
         <v>89370</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="L16">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -778,8 +930,14 @@
       <c r="C17">
         <v>75</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="H17">
+        <v>43000</v>
+      </c>
+      <c r="L17">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -790,13 +948,28 @@
         <v>40</v>
       </c>
       <c r="D18">
+        <v>19.5</v>
+      </c>
+      <c r="E18">
+        <v>20.79</v>
+      </c>
+      <c r="H18">
+        <v>41500</v>
+      </c>
+      <c r="I18">
+        <v>56165</v>
+      </c>
+      <c r="J18">
         <v>48000</v>
       </c>
-      <c r="E18">
+      <c r="K18">
         <v>86996</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="L18">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -807,13 +980,25 @@
         <v>45</v>
       </c>
       <c r="D19">
+        <v>18</v>
+      </c>
+      <c r="F19">
+        <v>33500</v>
+      </c>
+      <c r="H19">
+        <v>41000</v>
+      </c>
+      <c r="J19">
         <v>45275</v>
       </c>
-      <c r="E19">
+      <c r="K19">
         <v>46275</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="L19">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -823,8 +1008,26 @@
       <c r="C20">
         <v>250</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D20">
+        <v>24.38</v>
+      </c>
+      <c r="E20">
+        <v>25.64</v>
+      </c>
+      <c r="F20">
+        <v>41367</v>
+      </c>
+      <c r="H20">
+        <v>51039</v>
+      </c>
+      <c r="I20">
+        <v>73746</v>
+      </c>
+      <c r="L20">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -834,24 +1037,36 @@
       <c r="C21">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="L21">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>20</v>
       </c>
       <c r="C22">
         <v>100</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="H22">
+        <v>51763</v>
+      </c>
+      <c r="I22">
+        <v>77259</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>21</v>
       </c>
       <c r="C23">
         <v>48</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="L23">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -861,8 +1076,11 @@
       <c r="C24">
         <v>75</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="L24">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>23</v>
       </c>
@@ -873,13 +1091,28 @@
         <v>351</v>
       </c>
       <c r="D25">
+        <v>17.14</v>
+      </c>
+      <c r="E25">
+        <v>22.03</v>
+      </c>
+      <c r="H25">
+        <v>48315</v>
+      </c>
+      <c r="I25">
+        <v>81968</v>
+      </c>
+      <c r="J25">
         <v>55873</v>
       </c>
-      <c r="E25">
+      <c r="K25">
         <v>112197</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="L25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>24</v>
       </c>
@@ -890,13 +1123,28 @@
         <v>174</v>
       </c>
       <c r="D26">
+        <v>18.82</v>
+      </c>
+      <c r="E26">
+        <v>20.32</v>
+      </c>
+      <c r="H26">
+        <v>41000</v>
+      </c>
+      <c r="I26">
+        <v>42538</v>
+      </c>
+      <c r="J26">
         <v>53190</v>
       </c>
-      <c r="E26">
+      <c r="K26">
         <v>54190</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="L26">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>25</v>
       </c>
@@ -906,8 +1154,11 @@
       <c r="C27">
         <v>25</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="L27">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>26</v>
       </c>
@@ -918,13 +1169,25 @@
         <v>220</v>
       </c>
       <c r="D28">
+        <v>19</v>
+      </c>
+      <c r="E28">
+        <v>19.5</v>
+      </c>
+      <c r="H28">
+        <v>49000</v>
+      </c>
+      <c r="J28">
         <v>57000</v>
       </c>
-      <c r="E28">
+      <c r="K28">
         <v>58000</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="L28">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>27</v>
       </c>
@@ -934,8 +1197,29 @@
       <c r="C29">
         <v>85</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D29">
+        <v>19.62</v>
+      </c>
+      <c r="E29">
+        <v>29.15</v>
+      </c>
+      <c r="F29">
+        <v>42000</v>
+      </c>
+      <c r="G29">
+        <v>62416</v>
+      </c>
+      <c r="H29">
+        <v>44940</v>
+      </c>
+      <c r="I29">
+        <v>66785</v>
+      </c>
+      <c r="L29">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>28</v>
       </c>
@@ -945,14 +1229,29 @@
       <c r="C30">
         <v>300</v>
       </c>
-      <c r="D30">
+      <c r="F30">
+        <v>43348</v>
+      </c>
+      <c r="G30">
+        <v>48448</v>
+      </c>
+      <c r="H30">
+        <v>50998</v>
+      </c>
+      <c r="I30">
+        <v>81512</v>
+      </c>
+      <c r="J30">
         <v>61960</v>
       </c>
-      <c r="E30">
+      <c r="K30">
         <v>99052</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="L30">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>29</v>
       </c>
@@ -962,8 +1261,11 @@
       <c r="C31">
         <v>185</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="L31">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>30</v>
       </c>
@@ -973,14 +1275,20 @@
       <c r="C32">
         <v>18</v>
       </c>
-      <c r="D32">
+      <c r="H32">
+        <v>42000</v>
+      </c>
+      <c r="J32">
         <v>54000</v>
       </c>
-      <c r="E32">
+      <c r="K32">
         <v>55000</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="L32">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>31</v>
       </c>
@@ -990,14 +1298,26 @@
       <c r="C33">
         <v>80</v>
       </c>
-      <c r="D33">
+      <c r="F33">
+        <v>40258</v>
+      </c>
+      <c r="G33">
+        <v>44066</v>
+      </c>
+      <c r="H33">
+        <v>44796</v>
+      </c>
+      <c r="I33">
+        <v>69913</v>
+      </c>
+      <c r="J33">
         <v>95552</v>
       </c>
-      <c r="E33">
+      <c r="K33">
         <v>106660</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>32</v>
       </c>
@@ -1007,8 +1327,11 @@
       <c r="C34">
         <v>175</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="L34">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>33</v>
       </c>
@@ -1019,13 +1342,34 @@
         <v>250</v>
       </c>
       <c r="D35">
+        <v>22.25</v>
+      </c>
+      <c r="E35">
+        <v>26.81</v>
+      </c>
+      <c r="F35">
+        <v>46780</v>
+      </c>
+      <c r="G35">
+        <v>51656</v>
+      </c>
+      <c r="H35">
+        <v>51961</v>
+      </c>
+      <c r="I35">
+        <v>94988</v>
+      </c>
+      <c r="J35">
         <v>56085</v>
       </c>
-      <c r="E35">
+      <c r="K35">
         <v>101551</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="L35">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>34</v>
       </c>
@@ -1035,8 +1379,11 @@
       <c r="C36">
         <v>150</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="L36">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>35</v>
       </c>
@@ -1047,13 +1394,34 @@
         <v>583</v>
       </c>
       <c r="D37">
+        <v>23.44</v>
+      </c>
+      <c r="E37">
+        <v>27.13</v>
+      </c>
+      <c r="F37">
+        <v>48854</v>
+      </c>
+      <c r="G37">
+        <v>65469</v>
+      </c>
+      <c r="H37">
+        <v>53862</v>
+      </c>
+      <c r="I37">
         <v>72180</v>
       </c>
-      <c r="E37">
+      <c r="J37">
+        <v>72180</v>
+      </c>
+      <c r="K37">
         <v>96728</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="L37">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>36</v>
       </c>
@@ -1063,8 +1431,11 @@
       <c r="C38">
         <v>110</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="L38">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>37</v>
       </c>
@@ -1074,8 +1445,11 @@
       <c r="C39">
         <v>49</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="L39">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>38</v>
       </c>
@@ -1085,14 +1459,17 @@
       <c r="C40">
         <v>110</v>
       </c>
-      <c r="F40">
-        <v>30</v>
-      </c>
-      <c r="G40">
-        <v>62.04</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="D40">
+        <v>21.05</v>
+      </c>
+      <c r="E40">
+        <v>21.68</v>
+      </c>
+      <c r="L40">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>39</v>
       </c>
@@ -1103,13 +1480,28 @@
         <v>275</v>
       </c>
       <c r="D41">
+        <v>22.95</v>
+      </c>
+      <c r="E41">
+        <v>25.28</v>
+      </c>
+      <c r="H41">
+        <v>50542</v>
+      </c>
+      <c r="I41">
+        <v>85412</v>
+      </c>
+      <c r="J41">
         <v>59523</v>
       </c>
-      <c r="E41">
+      <c r="K41">
         <v>100589</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="L41">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>40</v>
       </c>
@@ -1117,16 +1509,22 @@
         <v>150</v>
       </c>
       <c r="D42">
+        <v>20.239999999999998</v>
+      </c>
+      <c r="H42">
+        <v>47239</v>
+      </c>
+      <c r="J42">
         <v>57428</v>
       </c>
-      <c r="E42">
+      <c r="K42">
         <v>58428</v>
       </c>
-      <c r="F42">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="L42">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>57</v>
       </c>
@@ -1136,16 +1534,31 @@
       <c r="C43">
         <v>70</v>
       </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="D43">
+        <v>26.99</v>
+      </c>
+      <c r="E43">
+        <v>33.08</v>
+      </c>
+      <c r="L43">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>41</v>
       </c>
       <c r="C44">
         <v>49</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="I44">
+        <v>85000</v>
+      </c>
+      <c r="L44">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>42</v>
       </c>
@@ -1155,14 +1568,23 @@
       <c r="C45">
         <v>132</v>
       </c>
-      <c r="D45">
+      <c r="H45">
+        <v>41890</v>
+      </c>
+      <c r="I45">
+        <v>49000</v>
+      </c>
+      <c r="J45">
         <v>51000</v>
       </c>
-      <c r="E45">
+      <c r="K45">
         <v>66000</v>
       </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="L45">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>43</v>
       </c>
@@ -1172,20 +1594,23 @@
       <c r="C46">
         <v>120</v>
       </c>
-      <c r="D46">
+      <c r="H46">
+        <v>49449</v>
+      </c>
+      <c r="I46">
+        <v>63536</v>
+      </c>
+      <c r="J46">
         <v>58185</v>
       </c>
-      <c r="E46">
+      <c r="K46">
         <v>82336</v>
       </c>
-      <c r="F46">
-        <v>25.75</v>
-      </c>
-      <c r="G46">
-        <v>55.98</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="L46">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>44</v>
       </c>
@@ -1195,14 +1620,20 @@
       <c r="C47">
         <v>350</v>
       </c>
-      <c r="D47">
+      <c r="H47">
+        <v>56061</v>
+      </c>
+      <c r="J47">
         <v>67766</v>
       </c>
-      <c r="E47">
+      <c r="K47">
         <v>68766</v>
       </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="L47">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>45</v>
       </c>
@@ -1212,8 +1643,17 @@
       <c r="C48">
         <v>174</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="H48">
+        <v>43756</v>
+      </c>
+      <c r="I48">
+        <v>58000</v>
+      </c>
+      <c r="L48">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>46</v>
       </c>
@@ -1223,8 +1663,14 @@
       <c r="C49">
         <v>90</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="H49">
+        <v>50000</v>
+      </c>
+      <c r="L49">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>47</v>
       </c>
@@ -1235,13 +1681,28 @@
         <v>471</v>
       </c>
       <c r="D50">
+        <v>22.37</v>
+      </c>
+      <c r="E50">
+        <v>26.34</v>
+      </c>
+      <c r="H50">
+        <v>49460</v>
+      </c>
+      <c r="I50">
+        <v>72147</v>
+      </c>
+      <c r="J50">
         <v>57294</v>
       </c>
-      <c r="E50">
+      <c r="K50">
         <v>82759</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="L50">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>48</v>
       </c>
@@ -1251,8 +1712,11 @@
       <c r="C51">
         <v>86</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="L51">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>49</v>
       </c>
@@ -1263,13 +1727,31 @@
         <v>325</v>
       </c>
       <c r="D52">
+        <v>22.45</v>
+      </c>
+      <c r="E52">
+        <v>26.63</v>
+      </c>
+      <c r="F52">
+        <v>40855</v>
+      </c>
+      <c r="G52">
+        <v>48160</v>
+      </c>
+      <c r="H52">
+        <v>51144</v>
+      </c>
+      <c r="I52">
+        <v>83472</v>
+      </c>
+      <c r="J52">
         <v>61417</v>
       </c>
-      <c r="E52">
+      <c r="K52">
         <v>106266</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>50</v>
       </c>
@@ -1279,8 +1761,11 @@
       <c r="C53">
         <v>50</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="L53">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>51</v>
       </c>
@@ -1290,28 +1775,49 @@
       <c r="C54">
         <v>125</v>
       </c>
-      <c r="D54">
+      <c r="H54">
+        <v>51355</v>
+      </c>
+      <c r="I54">
+        <v>66762</v>
+      </c>
+      <c r="J54">
         <v>62217</v>
       </c>
-      <c r="E54">
+      <c r="K54">
         <v>80882</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="L54">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>52</v>
       </c>
       <c r="B55">
         <v>35000</v>
       </c>
-      <c r="D55">
+      <c r="F55">
+        <v>40850</v>
+      </c>
+      <c r="G55">
+        <v>43012</v>
+      </c>
+      <c r="H55">
+        <v>47950</v>
+      </c>
+      <c r="J55">
         <v>53000</v>
       </c>
-      <c r="E55">
+      <c r="K55">
         <v>85750</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="L55">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>53</v>
       </c>
@@ -1321,8 +1827,29 @@
       <c r="C56">
         <v>75</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D56">
+        <v>17</v>
+      </c>
+      <c r="E56">
+        <v>19</v>
+      </c>
+      <c r="F56">
+        <v>30940</v>
+      </c>
+      <c r="G56">
+        <v>34580</v>
+      </c>
+      <c r="H56">
+        <v>25000</v>
+      </c>
+      <c r="I56">
+        <v>27000</v>
+      </c>
+      <c r="L56">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>54</v>
       </c>
@@ -1331,6 +1858,12 @@
       </c>
       <c r="C57">
         <v>250</v>
+      </c>
+      <c r="H57">
+        <v>48176</v>
+      </c>
+      <c r="L57">
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
-Update to histograms and functions
</commit_message>
<xml_diff>
--- a/SCLASurvey.xlsx
+++ b/SCLASurvey.xlsx
@@ -203,31 +203,31 @@
     <t>MeetingRoomCapacity</t>
   </si>
   <si>
-    <t>LibrarianIIISalLow</t>
-  </si>
-  <si>
-    <t>LibrarianIIISalHigh</t>
-  </si>
-  <si>
     <t>WeeklyHours</t>
   </si>
   <si>
-    <t>LibraryTraineeWageLow</t>
-  </si>
-  <si>
-    <t>LibraryTraineeWageHigh</t>
-  </si>
-  <si>
-    <t>LibraryTraineeSalLow</t>
-  </si>
-  <si>
-    <t>LibraryTraineeSalHigh</t>
-  </si>
-  <si>
-    <t>LibrarianISalLow</t>
-  </si>
-  <si>
-    <t>LibrarianISalHigh</t>
+    <t>LibTraineeWageLow</t>
+  </si>
+  <si>
+    <t>LibTraineeWageHigh</t>
+  </si>
+  <si>
+    <t>LibTraineeSalLow</t>
+  </si>
+  <si>
+    <t>LibTraineeSalHigh</t>
+  </si>
+  <si>
+    <t>LibISalLow</t>
+  </si>
+  <si>
+    <t>LibISalHigh</t>
+  </si>
+  <si>
+    <t>LibIIISalLow</t>
+  </si>
+  <si>
+    <t>LibIIISalHigh</t>
   </si>
 </sst>
 </file>
@@ -547,16 +547,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="H58" sqref="H58"/>
+    <sheetView tabSelected="1" topLeftCell="E41" workbookViewId="0">
+      <selection activeCell="K66" sqref="K66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="23.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="0" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="21.1796875" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="0" hidden="1" customWidth="1"/>
+    <col min="2" max="3" width="8.7265625" customWidth="1"/>
+    <col min="4" max="4" width="21.1796875" customWidth="1"/>
+    <col min="5" max="5" width="8.7265625" customWidth="1"/>
     <col min="8" max="8" width="14.54296875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15.453125" bestFit="1" customWidth="1"/>
   </cols>
@@ -572,31 +572,31 @@
         <v>58</v>
       </c>
       <c r="D1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F1" t="s">
         <v>62</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>63</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>64</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>65</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>66</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>67</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>59</v>
-      </c>
-      <c r="K1" t="s">
-        <v>60</v>
-      </c>
-      <c r="L1" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.35">
@@ -661,9 +661,6 @@
       <c r="J4">
         <v>48000</v>
       </c>
-      <c r="K4">
-        <v>49000</v>
-      </c>
       <c r="L4">
         <v>73</v>
       </c>
@@ -741,9 +738,6 @@
       <c r="J8">
         <v>71525</v>
       </c>
-      <c r="K8">
-        <v>72525</v>
-      </c>
       <c r="L8">
         <v>72</v>
       </c>
@@ -991,9 +985,6 @@
       <c r="J19">
         <v>45275</v>
       </c>
-      <c r="K19">
-        <v>46275</v>
-      </c>
       <c r="L19">
         <v>54</v>
       </c>
@@ -1137,9 +1128,6 @@
       <c r="J26">
         <v>53190</v>
       </c>
-      <c r="K26">
-        <v>54190</v>
-      </c>
       <c r="L26">
         <v>62</v>
       </c>
@@ -1180,9 +1168,6 @@
       <c r="J28">
         <v>57000</v>
       </c>
-      <c r="K28">
-        <v>58000</v>
-      </c>
       <c r="L28">
         <v>67</v>
       </c>
@@ -1281,9 +1266,6 @@
       <c r="J32">
         <v>54000</v>
       </c>
-      <c r="K32">
-        <v>55000</v>
-      </c>
       <c r="L32">
         <v>65</v>
       </c>
@@ -1517,9 +1499,6 @@
       <c r="J42">
         <v>57428</v>
       </c>
-      <c r="K42">
-        <v>58428</v>
-      </c>
       <c r="L42">
         <v>66</v>
       </c>
@@ -1625,9 +1604,6 @@
       </c>
       <c r="J47">
         <v>67766</v>
-      </c>
-      <c r="K47">
-        <v>68766</v>
       </c>
       <c r="L47">
         <v>70</v>

</xml_diff>

<commit_message>
Partially through completion of salary tab.
</commit_message>
<xml_diff>
--- a/SCLASurvey.xlsx
+++ b/SCLASurvey.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4186" uniqueCount="2023">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4188" uniqueCount="2039">
   <si>
     <t xml:space="preserve">Director </t>
   </si>
@@ -5683,18 +5683,6 @@
     <t>Annual Leave Days_Paid Holidays</t>
   </si>
   <si>
-    <t>Library Trainee_Part Time_Max Salary</t>
-  </si>
-  <si>
-    <t>Librarian/Librarian I_Part Time_Max Salary</t>
-  </si>
-  <si>
-    <t>Librarian II _Part Time_ Max Salary</t>
-  </si>
-  <si>
-    <t>Librarian III _Part Time_ Max Salary</t>
-  </si>
-  <si>
     <t>Clerk/Library Clerk_Part Time_Max Salary</t>
   </si>
   <si>
@@ -5842,9 +5830,6 @@
     <t>StaffCt_Administration_FT</t>
   </si>
   <si>
-    <t>StaffCt_Administration _PT</t>
-  </si>
-  <si>
     <t>StaffCt_Circulation_FT</t>
   </si>
   <si>
@@ -5893,9 +5878,6 @@
     <t>LoanPer_New_DVDs_Non-Fiction</t>
   </si>
   <si>
-    <t>LoanPer_Regular_DVDs_Fiction</t>
-  </si>
-  <si>
     <t>LoanPer_Regular_DVDs_Non-Fiction</t>
   </si>
   <si>
@@ -5935,18 +5917,6 @@
     <t>Fine_Books_Juvenile_Max</t>
   </si>
   <si>
-    <t>Fine_New_Books_Adult_Daily</t>
-  </si>
-  <si>
-    <t>Fine_New_Books_Adult_Max</t>
-  </si>
-  <si>
-    <t>Fine_New_Books_Juvenile_Daily</t>
-  </si>
-  <si>
-    <t>Fine_New_Books_Juvenile_Max</t>
-  </si>
-  <si>
     <t>Fine_Audiobooks_Adult_Daily</t>
   </si>
   <si>
@@ -6007,9 +5977,6 @@
     <t>Fine_Music_Juvenile_Max</t>
   </si>
   <si>
-    <t>Fine_Adult_Software_Daily</t>
-  </si>
-  <si>
     <t>Fine_Software_Adult_Max</t>
   </si>
   <si>
@@ -6070,9 +6037,6 @@
     <t>LoanPer_New_Audiobooks</t>
   </si>
   <si>
-    <t>LoanPer_Regular_Audiobook</t>
-  </si>
-  <si>
     <t>LoanPer_New_Digital_Audiobooks</t>
   </si>
   <si>
@@ -6095,6 +6059,90 @@
   </si>
   <si>
     <t>LoanPer_Regular_Videogames</t>
+  </si>
+  <si>
+    <t>StaffCt_Administration_PT</t>
+  </si>
+  <si>
+    <t>LoanPer_Regular_Audiobooks</t>
+  </si>
+  <si>
+    <t>LoanPer_Regular_DVDs-Fiction</t>
+  </si>
+  <si>
+    <t>Fine_Software_Adult_Daily</t>
+  </si>
+  <si>
+    <t>Fine_New Books_Adult_Daily</t>
+  </si>
+  <si>
+    <t>Fine_New Books_Adult_Max</t>
+  </si>
+  <si>
+    <t>Fine_New Books_Juvenile_Daily</t>
+  </si>
+  <si>
+    <t>Fine_New Books_Juvenile_Max</t>
+  </si>
+  <si>
+    <t>MinSal_Librarian Trainee_PT</t>
+  </si>
+  <si>
+    <t>MaxSal_Librarian Trainee_PT</t>
+  </si>
+  <si>
+    <t>MaxSal_Librarian Trainee_FT</t>
+  </si>
+  <si>
+    <t>MinSal_Librarian Trainee_FT</t>
+  </si>
+  <si>
+    <t>MinSal_Librarian I_FT</t>
+  </si>
+  <si>
+    <t>MaxSal_Librarian I_FT</t>
+  </si>
+  <si>
+    <t>MinSal_Librarian I_PT</t>
+  </si>
+  <si>
+    <t>MaxSal_Librarian I_PT</t>
+  </si>
+  <si>
+    <t>MinSal_Librarian II_FT</t>
+  </si>
+  <si>
+    <t>MaxSal_Librarian II_FT</t>
+  </si>
+  <si>
+    <t>MinSal_Librarian II_PT</t>
+  </si>
+  <si>
+    <t>MaxSal_Librarian II_PT</t>
+  </si>
+  <si>
+    <t>MinSal_Librarian III_FT</t>
+  </si>
+  <si>
+    <t>MaxSal_Librarian III_FT</t>
+  </si>
+  <si>
+    <t>MinSal_Librarian III_PT</t>
+  </si>
+  <si>
+    <t>MaxSal_Librarian III_PT</t>
+  </si>
+  <si>
+    <t>MinSal_Librarian IV_FT</t>
+  </si>
+  <si>
+    <t>MaxSal_Librarian IV_FT</t>
+  </si>
+  <si>
+    <t>MinSal_Librarian IV_PT</t>
+  </si>
+  <si>
+    <t>MaxSal_Librarian IV_PT</t>
   </si>
 </sst>
 </file>
@@ -6866,10 +6914,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:GJ82"/>
+  <dimension ref="A2:GL82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AR1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="BB1" sqref="BB1:BB1048576"/>
+    <sheetView tabSelected="1" topLeftCell="EJ1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="EP3" sqref="EP3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6917,7 +6965,7 @@
     <col min="140" max="140" width="31.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:192" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:194" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1880</v>
       </c>
@@ -6925,277 +6973,277 @@
         <v>1879</v>
       </c>
       <c r="C2" t="s">
+        <v>1928</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1929</v>
+      </c>
+      <c r="E2" t="s">
+        <v>1930</v>
+      </c>
+      <c r="F2" t="s">
+        <v>1931</v>
+      </c>
+      <c r="G2" t="s">
         <v>1932</v>
       </c>
-      <c r="D2" t="s">
+      <c r="H2" t="s">
         <v>1933</v>
       </c>
-      <c r="E2" t="s">
+      <c r="I2" t="s">
+        <v>2011</v>
+      </c>
+      <c r="J2" t="s">
+        <v>1994</v>
+      </c>
+      <c r="K2" t="s">
+        <v>1995</v>
+      </c>
+      <c r="L2" t="s">
+        <v>1996</v>
+      </c>
+      <c r="M2" t="s">
+        <v>1997</v>
+      </c>
+      <c r="N2" t="s">
         <v>1934</v>
       </c>
-      <c r="F2" t="s">
+      <c r="O2" t="s">
         <v>1935</v>
       </c>
-      <c r="G2" t="s">
+      <c r="P2" t="s">
         <v>1936</v>
       </c>
-      <c r="H2" t="s">
+      <c r="Q2" t="s">
         <v>1937</v>
       </c>
-      <c r="I2" t="s">
+      <c r="R2" t="s">
+        <v>1998</v>
+      </c>
+      <c r="S2" t="s">
+        <v>1999</v>
+      </c>
+      <c r="T2" t="s">
+        <v>2000</v>
+      </c>
+      <c r="U2" t="s">
+        <v>2001</v>
+      </c>
+      <c r="V2" t="s">
         <v>1938</v>
       </c>
-      <c r="J2" t="s">
+      <c r="W2" t="s">
+        <v>1939</v>
+      </c>
+      <c r="X2" t="s">
+        <v>1940</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>1941</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>1942</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>1943</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>1944</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>1945</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>1946</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>1947</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>2002</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>2012</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>1948</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>1949</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>2013</v>
+      </c>
+      <c r="AK2" t="s">
+        <v>1950</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>1951</v>
+      </c>
+      <c r="AM2" t="s">
+        <v>1952</v>
+      </c>
+      <c r="AN2" t="s">
+        <v>1953</v>
+      </c>
+      <c r="AO2" t="s">
+        <v>1954</v>
+      </c>
+      <c r="AP2" t="s">
+        <v>1955</v>
+      </c>
+      <c r="AQ2" t="s">
+        <v>1956</v>
+      </c>
+      <c r="AR2" t="s">
+        <v>1957</v>
+      </c>
+      <c r="AS2" t="s">
+        <v>1958</v>
+      </c>
+      <c r="AT2" t="s">
+        <v>2006</v>
+      </c>
+      <c r="AU2" t="s">
         <v>2005</v>
       </c>
-      <c r="K2" t="s">
-        <v>2006</v>
-      </c>
-      <c r="L2" t="s">
+      <c r="AV2" t="s">
         <v>2007</v>
       </c>
-      <c r="M2" t="s">
+      <c r="AW2" t="s">
         <v>2008</v>
       </c>
-      <c r="N2" t="s">
-        <v>1939</v>
-      </c>
-      <c r="O2" t="s">
-        <v>1940</v>
-      </c>
-      <c r="P2" t="s">
-        <v>1941</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>1942</v>
-      </c>
-      <c r="R2" t="s">
+      <c r="AX2" t="s">
         <v>2009</v>
       </c>
-      <c r="S2" t="s">
+      <c r="AY2" t="s">
         <v>2010</v>
       </c>
-      <c r="T2" t="s">
-        <v>2011</v>
-      </c>
-      <c r="U2" t="s">
-        <v>2012</v>
-      </c>
-      <c r="V2" t="s">
-        <v>1943</v>
-      </c>
-      <c r="W2" t="s">
-        <v>1944</v>
-      </c>
-      <c r="X2" t="s">
-        <v>1945</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>1946</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>1947</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>1948</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>1949</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>1950</v>
-      </c>
-      <c r="AD2" t="s">
-        <v>1951</v>
-      </c>
-      <c r="AE2" t="s">
-        <v>1952</v>
-      </c>
-      <c r="AF2" t="s">
-        <v>2013</v>
-      </c>
-      <c r="AG2" t="s">
+      <c r="AZ2" t="s">
+        <v>2003</v>
+      </c>
+      <c r="BA2" t="s">
+        <v>2004</v>
+      </c>
+      <c r="BB2" t="s">
+        <v>1959</v>
+      </c>
+      <c r="BC2" t="s">
+        <v>1960</v>
+      </c>
+      <c r="BD2" t="s">
+        <v>1961</v>
+      </c>
+      <c r="BE2" t="s">
+        <v>1962</v>
+      </c>
+      <c r="BF2" t="s">
+        <v>2015</v>
+      </c>
+      <c r="BG2" t="s">
+        <v>2016</v>
+      </c>
+      <c r="BH2" t="s">
+        <v>2017</v>
+      </c>
+      <c r="BI2" t="s">
+        <v>2018</v>
+      </c>
+      <c r="BJ2" t="s">
+        <v>1963</v>
+      </c>
+      <c r="BK2" t="s">
+        <v>1964</v>
+      </c>
+      <c r="BL2" t="s">
+        <v>1965</v>
+      </c>
+      <c r="BM2" t="s">
+        <v>1966</v>
+      </c>
+      <c r="BN2" t="s">
+        <v>1967</v>
+      </c>
+      <c r="BO2" t="s">
+        <v>1968</v>
+      </c>
+      <c r="BP2" t="s">
+        <v>1969</v>
+      </c>
+      <c r="BQ2" t="s">
+        <v>1970</v>
+      </c>
+      <c r="BR2" t="s">
+        <v>1971</v>
+      </c>
+      <c r="BS2" t="s">
+        <v>1972</v>
+      </c>
+      <c r="BT2" t="s">
+        <v>1973</v>
+      </c>
+      <c r="BU2" t="s">
+        <v>1974</v>
+      </c>
+      <c r="BV2" t="s">
+        <v>1975</v>
+      </c>
+      <c r="BW2" t="s">
+        <v>1976</v>
+      </c>
+      <c r="BX2" t="s">
+        <v>1977</v>
+      </c>
+      <c r="BY2" t="s">
+        <v>1978</v>
+      </c>
+      <c r="BZ2" t="s">
+        <v>1979</v>
+      </c>
+      <c r="CA2" t="s">
+        <v>1980</v>
+      </c>
+      <c r="CB2" t="s">
+        <v>1981</v>
+      </c>
+      <c r="CC2" t="s">
+        <v>1982</v>
+      </c>
+      <c r="CD2" t="s">
         <v>2014</v>
       </c>
-      <c r="AH2" t="s">
-        <v>1953</v>
-      </c>
-      <c r="AI2" t="s">
-        <v>1954</v>
-      </c>
-      <c r="AJ2" t="s">
-        <v>1955</v>
-      </c>
-      <c r="AK2" t="s">
-        <v>1956</v>
-      </c>
-      <c r="AL2" t="s">
-        <v>1957</v>
-      </c>
-      <c r="AM2" t="s">
-        <v>1958</v>
-      </c>
-      <c r="AN2" t="s">
-        <v>1959</v>
-      </c>
-      <c r="AO2" t="s">
-        <v>1960</v>
-      </c>
-      <c r="AP2" t="s">
-        <v>1961</v>
-      </c>
-      <c r="AQ2" t="s">
-        <v>1962</v>
-      </c>
-      <c r="AR2" t="s">
-        <v>1963</v>
-      </c>
-      <c r="AS2" t="s">
-        <v>1964</v>
-      </c>
-      <c r="AT2" t="s">
-        <v>2018</v>
-      </c>
-      <c r="AU2" t="s">
-        <v>2017</v>
-      </c>
-      <c r="AV2" t="s">
-        <v>2019</v>
-      </c>
-      <c r="AW2" t="s">
-        <v>2020</v>
-      </c>
-      <c r="AX2" t="s">
-        <v>2021</v>
-      </c>
-      <c r="AY2" t="s">
-        <v>2022</v>
-      </c>
-      <c r="AZ2" t="s">
-        <v>2015</v>
-      </c>
-      <c r="BA2" t="s">
-        <v>2016</v>
-      </c>
-      <c r="BB2" t="s">
-        <v>1965</v>
-      </c>
-      <c r="BC2" t="s">
-        <v>1966</v>
-      </c>
-      <c r="BD2" t="s">
-        <v>1967</v>
-      </c>
-      <c r="BE2" t="s">
-        <v>1968</v>
-      </c>
-      <c r="BF2" t="s">
-        <v>1969</v>
-      </c>
-      <c r="BG2" t="s">
-        <v>1970</v>
-      </c>
-      <c r="BH2" t="s">
-        <v>1971</v>
-      </c>
-      <c r="BI2" t="s">
-        <v>1972</v>
-      </c>
-      <c r="BJ2" t="s">
-        <v>1973</v>
-      </c>
-      <c r="BK2" t="s">
-        <v>1974</v>
-      </c>
-      <c r="BL2" t="s">
-        <v>1975</v>
-      </c>
-      <c r="BM2" t="s">
-        <v>1976</v>
-      </c>
-      <c r="BN2" t="s">
-        <v>1977</v>
-      </c>
-      <c r="BO2" t="s">
-        <v>1978</v>
-      </c>
-      <c r="BP2" t="s">
-        <v>1979</v>
-      </c>
-      <c r="BQ2" t="s">
-        <v>1980</v>
-      </c>
-      <c r="BR2" t="s">
-        <v>1981</v>
-      </c>
-      <c r="BS2" t="s">
-        <v>1982</v>
-      </c>
-      <c r="BT2" t="s">
+      <c r="CE2" t="s">
         <v>1983</v>
       </c>
-      <c r="BU2" t="s">
+      <c r="CF2" t="s">
         <v>1984</v>
       </c>
-      <c r="BV2" t="s">
+      <c r="CG2" t="s">
         <v>1985</v>
       </c>
-      <c r="BW2" t="s">
+      <c r="CH2" t="s">
         <v>1986</v>
       </c>
-      <c r="BX2" t="s">
+      <c r="CI2" t="s">
         <v>1987</v>
       </c>
-      <c r="BY2" t="s">
+      <c r="CJ2" t="s">
         <v>1988</v>
       </c>
-      <c r="BZ2" t="s">
+      <c r="CK2" t="s">
         <v>1989</v>
       </c>
-      <c r="CA2" t="s">
+      <c r="CL2" t="s">
         <v>1990</v>
       </c>
-      <c r="CB2" t="s">
+      <c r="CM2" t="s">
         <v>1991</v>
       </c>
-      <c r="CC2" t="s">
+      <c r="CN2" t="s">
         <v>1992</v>
       </c>
-      <c r="CD2" t="s">
+      <c r="CO2" t="s">
         <v>1993</v>
-      </c>
-      <c r="CE2" t="s">
-        <v>1994</v>
-      </c>
-      <c r="CF2" t="s">
-        <v>1995</v>
-      </c>
-      <c r="CG2" t="s">
-        <v>1996</v>
-      </c>
-      <c r="CH2" t="s">
-        <v>1997</v>
-      </c>
-      <c r="CI2" t="s">
-        <v>1998</v>
-      </c>
-      <c r="CJ2" t="s">
-        <v>1999</v>
-      </c>
-      <c r="CK2" t="s">
-        <v>2000</v>
-      </c>
-      <c r="CL2" t="s">
-        <v>2001</v>
-      </c>
-      <c r="CM2" t="s">
-        <v>2002</v>
-      </c>
-      <c r="CN2" t="s">
-        <v>2003</v>
-      </c>
-      <c r="CO2" t="s">
-        <v>2004</v>
       </c>
       <c r="CP2" t="s">
         <v>23</v>
@@ -7300,157 +7348,163 @@
         <v>557</v>
       </c>
       <c r="DX2" t="s">
-        <v>575</v>
+        <v>2022</v>
       </c>
       <c r="DY2" t="s">
-        <v>577</v>
+        <v>2021</v>
       </c>
       <c r="DZ2" t="s">
-        <v>1133</v>
+        <v>2019</v>
       </c>
       <c r="EA2" t="s">
+        <v>2020</v>
+      </c>
+      <c r="EB2" t="s">
+        <v>2023</v>
+      </c>
+      <c r="EC2" t="s">
+        <v>2024</v>
+      </c>
+      <c r="ED2" t="s">
+        <v>2025</v>
+      </c>
+      <c r="EE2" t="s">
+        <v>2026</v>
+      </c>
+      <c r="EF2" t="s">
+        <v>2027</v>
+      </c>
+      <c r="EG2" t="s">
+        <v>2028</v>
+      </c>
+      <c r="EH2" t="s">
+        <v>2029</v>
+      </c>
+      <c r="EI2" t="s">
+        <v>2030</v>
+      </c>
+      <c r="EJ2" t="s">
+        <v>2031</v>
+      </c>
+      <c r="EK2" t="s">
+        <v>2032</v>
+      </c>
+      <c r="EL2" t="s">
+        <v>2033</v>
+      </c>
+      <c r="EM2" t="s">
+        <v>2034</v>
+      </c>
+      <c r="EN2" t="s">
+        <v>2035</v>
+      </c>
+      <c r="EO2" t="s">
+        <v>2036</v>
+      </c>
+      <c r="EP2" t="s">
+        <v>2037</v>
+      </c>
+      <c r="EQ2" t="s">
+        <v>2038</v>
+      </c>
+      <c r="ER2" t="s">
+        <v>659</v>
+      </c>
+      <c r="ES2" t="s">
+        <v>660</v>
+      </c>
+      <c r="ET2" t="s">
+        <v>560</v>
+      </c>
+      <c r="EU2" t="s">
         <v>1885</v>
       </c>
-      <c r="EB2" t="s">
-        <v>580</v>
-      </c>
-      <c r="EC2" t="s">
-        <v>581</v>
-      </c>
-      <c r="ED2" t="s">
-        <v>582</v>
-      </c>
-      <c r="EE2" t="s">
+      <c r="EV2" t="s">
+        <v>662</v>
+      </c>
+      <c r="EW2" t="s">
+        <v>663</v>
+      </c>
+      <c r="EX2" t="s">
+        <v>665</v>
+      </c>
+      <c r="EY2" t="s">
         <v>1886</v>
       </c>
-      <c r="EF2" t="s">
-        <v>585</v>
-      </c>
-      <c r="EG2" t="s">
-        <v>637</v>
-      </c>
-      <c r="EH2" t="s">
-        <v>639</v>
-      </c>
-      <c r="EI2" t="s">
+      <c r="EZ2" t="s">
+        <v>668</v>
+      </c>
+      <c r="FA2" t="s">
+        <v>669</v>
+      </c>
+      <c r="FB2" t="s">
+        <v>729</v>
+      </c>
+      <c r="FC2" t="s">
+        <v>730</v>
+      </c>
+      <c r="FD2" t="s">
+        <v>872</v>
+      </c>
+      <c r="FE2" t="s">
         <v>1887</v>
       </c>
-      <c r="EJ2" t="s">
-        <v>642</v>
-      </c>
-      <c r="EK2" t="s">
-        <v>643</v>
-      </c>
-      <c r="EL2" t="s">
-        <v>645</v>
-      </c>
-      <c r="EM2" t="s">
+      <c r="FF2" t="s">
+        <v>887</v>
+      </c>
+      <c r="FG2" t="s">
+        <v>888</v>
+      </c>
+      <c r="FH2" t="s">
+        <v>597</v>
+      </c>
+      <c r="FI2" t="s">
         <v>1888</v>
       </c>
-      <c r="EN2" t="s">
-        <v>648</v>
-      </c>
-      <c r="EO2" t="s">
-        <v>649</v>
-      </c>
-      <c r="EP2" t="s">
-        <v>659</v>
-      </c>
-      <c r="EQ2" t="s">
-        <v>660</v>
-      </c>
-      <c r="ER2" t="s">
-        <v>560</v>
-      </c>
-      <c r="ES2" t="s">
+      <c r="FJ2" t="s">
+        <v>598</v>
+      </c>
+      <c r="FK2" t="s">
+        <v>890</v>
+      </c>
+      <c r="FL2" t="s">
+        <v>894</v>
+      </c>
+      <c r="FM2" t="s">
+        <v>895</v>
+      </c>
+      <c r="FN2" t="s">
+        <v>601</v>
+      </c>
+      <c r="FO2" t="s">
+        <v>602</v>
+      </c>
+      <c r="FP2" t="s">
+        <v>943</v>
+      </c>
+      <c r="FQ2" t="s">
+        <v>944</v>
+      </c>
+      <c r="FR2" t="s">
+        <v>609</v>
+      </c>
+      <c r="FS2" t="s">
+        <v>976</v>
+      </c>
+      <c r="FT2" t="s">
+        <v>981</v>
+      </c>
+      <c r="FU2" t="s">
+        <v>982</v>
+      </c>
+      <c r="FV2" t="s">
+        <v>610</v>
+      </c>
+      <c r="FW2" t="s">
         <v>1889</v>
       </c>
-      <c r="ET2" t="s">
-        <v>662</v>
-      </c>
-      <c r="EU2" t="s">
-        <v>663</v>
-      </c>
-      <c r="EV2" t="s">
-        <v>665</v>
-      </c>
-      <c r="EW2" t="s">
-        <v>1890</v>
-      </c>
-      <c r="EX2" t="s">
-        <v>668</v>
-      </c>
-      <c r="EY2" t="s">
-        <v>669</v>
-      </c>
-      <c r="EZ2" t="s">
-        <v>729</v>
-      </c>
-      <c r="FA2" t="s">
-        <v>730</v>
-      </c>
-      <c r="FB2" t="s">
-        <v>872</v>
-      </c>
-      <c r="FC2" t="s">
-        <v>1891</v>
-      </c>
-      <c r="FD2" t="s">
-        <v>887</v>
-      </c>
-      <c r="FE2" t="s">
-        <v>888</v>
-      </c>
-      <c r="FF2" t="s">
-        <v>597</v>
-      </c>
-      <c r="FG2" t="s">
-        <v>1892</v>
-      </c>
-      <c r="FH2" t="s">
-        <v>598</v>
-      </c>
-      <c r="FI2" t="s">
-        <v>890</v>
-      </c>
-      <c r="FJ2" t="s">
-        <v>894</v>
-      </c>
-      <c r="FK2" t="s">
-        <v>895</v>
-      </c>
-      <c r="FL2" t="s">
-        <v>601</v>
-      </c>
-      <c r="FM2" t="s">
-        <v>602</v>
-      </c>
-      <c r="FN2" t="s">
-        <v>943</v>
-      </c>
-      <c r="FO2" t="s">
-        <v>944</v>
-      </c>
-      <c r="FP2" t="s">
-        <v>609</v>
-      </c>
-      <c r="FQ2" t="s">
-        <v>976</v>
-      </c>
-      <c r="FR2" t="s">
-        <v>981</v>
-      </c>
-      <c r="FS2" t="s">
-        <v>982</v>
-      </c>
-      <c r="FT2" t="s">
-        <v>610</v>
-      </c>
-      <c r="FU2" t="s">
-        <v>1893</v>
-      </c>
     </row>
-    <row r="3" spans="1:192" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:194" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>1844</v>
       </c>
@@ -7701,47 +7755,47 @@
       <c r="EK3">
         <v>62722.400000000001</v>
       </c>
-      <c r="EP3">
+      <c r="ER3">
         <v>28072.27</v>
       </c>
-      <c r="EQ3">
+      <c r="ES3">
         <v>28831.65</v>
       </c>
-      <c r="ER3">
+      <c r="ET3">
         <v>13.13</v>
       </c>
-      <c r="ES3">
+      <c r="EU3">
         <v>13.92</v>
       </c>
-      <c r="ET3">
+      <c r="EV3">
         <v>34234.49</v>
       </c>
-      <c r="EU3">
+      <c r="EW3">
         <v>35753.25</v>
       </c>
-      <c r="EZ3">
+      <c r="FB3">
         <v>49982.35</v>
       </c>
-      <c r="FA3">
+      <c r="FC3">
         <v>49982.35</v>
       </c>
-      <c r="FG3">
+      <c r="FI3">
         <v>13.13</v>
       </c>
-      <c r="FR3">
+      <c r="FT3">
         <v>82000</v>
       </c>
-      <c r="FS3">
+      <c r="FU3">
         <v>82000</v>
       </c>
-      <c r="FT3">
+      <c r="FV3">
         <v>8.92</v>
       </c>
-      <c r="FU3">
+      <c r="FW3">
         <v>13.3</v>
       </c>
     </row>
-    <row r="4" spans="1:192" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:194" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>1846</v>
       </c>
@@ -8099,44 +8153,44 @@
       <c r="EK4">
         <v>75000</v>
       </c>
-      <c r="ER4">
+      <c r="ET4">
         <v>11.5</v>
       </c>
-      <c r="ES4">
+      <c r="EU4">
         <v>26</v>
       </c>
-      <c r="ET4">
+      <c r="EV4">
         <v>51000</v>
       </c>
-      <c r="EU4">
+      <c r="EW4">
         <v>53000</v>
       </c>
-      <c r="FH4">
+      <c r="FJ4">
         <v>39000</v>
       </c>
-      <c r="FI4">
+      <c r="FK4">
         <v>45000</v>
       </c>
-      <c r="FP4">
+      <c r="FR4">
         <v>65000</v>
       </c>
-      <c r="FQ4">
+      <c r="FS4">
         <v>75000</v>
       </c>
-      <c r="FR4">
+      <c r="FT4">
         <v>110000</v>
       </c>
-      <c r="FS4">
+      <c r="FU4">
         <v>120000</v>
       </c>
-      <c r="FT4">
+      <c r="FV4">
         <v>9</v>
       </c>
-      <c r="FU4">
+      <c r="FW4">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:192" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:194" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>1067</v>
       </c>
@@ -8458,74 +8512,74 @@
       <c r="EK5">
         <v>58792</v>
       </c>
-      <c r="EP5">
+      <c r="ER5">
         <v>31666</v>
       </c>
-      <c r="EQ5">
+      <c r="ES5">
         <v>31666</v>
       </c>
-      <c r="ER5">
+      <c r="ET5">
         <v>15.21</v>
       </c>
-      <c r="ES5">
+      <c r="EU5">
         <v>15.21</v>
       </c>
-      <c r="ET5">
+      <c r="EV5">
         <v>34240</v>
       </c>
-      <c r="EU5">
+      <c r="EW5">
         <v>34240</v>
       </c>
-      <c r="EX5">
+      <c r="EZ5">
         <v>36637</v>
       </c>
-      <c r="EY5">
+      <c r="FA5">
         <v>36637</v>
       </c>
-      <c r="FB5">
+      <c r="FD5">
         <v>16</v>
       </c>
-      <c r="FC5">
+      <c r="FE5">
         <v>16</v>
       </c>
-      <c r="FD5">
+      <c r="FF5">
         <v>32618</v>
       </c>
-      <c r="FE5">
+      <c r="FG5">
         <v>32618</v>
       </c>
-      <c r="FF5">
+      <c r="FH5">
         <v>15.59</v>
       </c>
-      <c r="FH5">
+      <c r="FJ5">
         <v>33275</v>
       </c>
-      <c r="FI5">
+      <c r="FK5">
         <v>33275</v>
       </c>
-      <c r="FJ5">
+      <c r="FL5">
         <v>34005</v>
       </c>
-      <c r="FK5">
+      <c r="FM5">
         <v>34005</v>
       </c>
-      <c r="GD5" t="s">
+      <c r="GF5" t="s">
         <v>1843</v>
       </c>
-      <c r="GG5" t="s">
+      <c r="GI5" t="s">
         <v>1867</v>
       </c>
-      <c r="GH5" t="s">
+      <c r="GJ5" t="s">
         <v>508</v>
       </c>
-      <c r="GI5" t="s">
+      <c r="GK5" t="s">
         <v>1869</v>
       </c>
-      <c r="GJ5" s="46" t="s">
+      <c r="GL5" s="46" t="s">
         <v>1873</v>
       </c>
     </row>
-    <row r="6" spans="1:192" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:194" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>1847</v>
       </c>
@@ -8799,41 +8853,41 @@
       <c r="EG6">
         <v>79789</v>
       </c>
-      <c r="EP6">
+      <c r="ER6">
         <v>39166</v>
       </c>
-      <c r="EQ6">
+      <c r="ES6">
         <v>46392</v>
       </c>
-      <c r="ER6">
+      <c r="ET6">
         <v>13520</v>
       </c>
-      <c r="ES6">
+      <c r="EU6">
         <v>19583</v>
       </c>
-      <c r="FR6">
+      <c r="FT6">
         <v>122000</v>
       </c>
-      <c r="FS6">
+      <c r="FU6">
         <v>122000</v>
       </c>
-      <c r="GD6" t="s">
+      <c r="GF6" t="s">
         <v>1879</v>
       </c>
-      <c r="GG6" t="s">
+      <c r="GI6" t="s">
         <v>414</v>
       </c>
-      <c r="GH6" t="s">
+      <c r="GJ6" t="s">
         <v>509</v>
       </c>
-      <c r="GI6" t="s">
+      <c r="GK6" t="s">
         <v>1870</v>
       </c>
-      <c r="GJ6" s="46" t="s">
+      <c r="GL6" s="46" t="s">
         <v>1874</v>
       </c>
     </row>
-    <row r="7" spans="1:192" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:194" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>1848</v>
       </c>
@@ -9056,68 +9110,68 @@
       <c r="EM7">
         <v>33.659999999999997</v>
       </c>
-      <c r="EP7">
+      <c r="ER7">
         <v>25613</v>
       </c>
-      <c r="EQ7">
+      <c r="ES7">
         <v>40388</v>
       </c>
-      <c r="ER7">
+      <c r="ET7">
         <v>10</v>
       </c>
-      <c r="ES7">
+      <c r="EU7">
         <v>19.8</v>
       </c>
-      <c r="ET7">
+      <c r="EV7">
         <v>28408</v>
       </c>
-      <c r="EU7">
+      <c r="EW7">
         <v>44797</v>
       </c>
-      <c r="EX7">
+      <c r="EZ7">
         <v>40482</v>
       </c>
-      <c r="EY7">
+      <c r="FA7">
         <v>48067</v>
       </c>
-      <c r="FD7">
+      <c r="FF7">
         <v>30757</v>
       </c>
-      <c r="FE7">
+      <c r="FG7">
         <v>48500</v>
       </c>
-      <c r="FF7">
+      <c r="FH7">
         <v>10.199999999999999</v>
       </c>
-      <c r="FG7">
+      <c r="FI7">
         <v>14.57</v>
       </c>
-      <c r="FH7">
+      <c r="FJ7">
         <v>35153</v>
       </c>
-      <c r="FI7">
+      <c r="FK7">
         <v>50703</v>
       </c>
-      <c r="FT7">
+      <c r="FV7">
         <v>8.5</v>
       </c>
-      <c r="FU7">
+      <c r="FW7">
         <v>8.75</v>
       </c>
-      <c r="GG7" t="s">
+      <c r="GI7" t="s">
         <v>415</v>
       </c>
-      <c r="GH7" t="s">
+      <c r="GJ7" t="s">
         <v>4</v>
       </c>
-      <c r="GI7" t="s">
+      <c r="GK7" t="s">
         <v>1871</v>
       </c>
-      <c r="GJ7" t="s">
+      <c r="GL7" t="s">
         <v>1875</v>
       </c>
     </row>
-    <row r="8" spans="1:192" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:194" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>1849</v>
       </c>
@@ -9365,44 +9419,44 @@
       <c r="EK8">
         <v>58708</v>
       </c>
-      <c r="ET8">
+      <c r="EV8">
         <v>33722</v>
       </c>
-      <c r="EU8">
+      <c r="EW8">
         <v>48750</v>
       </c>
-      <c r="FB8">
+      <c r="FD8">
         <v>16.55</v>
       </c>
-      <c r="FC8">
+      <c r="FE8">
         <v>19.14</v>
       </c>
-      <c r="FR8">
+      <c r="FT8">
         <v>84318</v>
       </c>
-      <c r="FS8">
+      <c r="FU8">
         <v>121914</v>
       </c>
-      <c r="FT8">
+      <c r="FV8">
         <v>9.02</v>
       </c>
-      <c r="FU8">
+      <c r="FW8">
         <v>9.91</v>
       </c>
-      <c r="GG8" t="s">
+      <c r="GI8" t="s">
         <v>416</v>
       </c>
-      <c r="GH8" t="s">
+      <c r="GJ8" t="s">
         <v>5</v>
       </c>
-      <c r="GI8" t="s">
+      <c r="GK8" t="s">
         <v>1872</v>
       </c>
-      <c r="GJ8" t="s">
+      <c r="GL8" t="s">
         <v>1876</v>
       </c>
     </row>
-    <row r="9" spans="1:192" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:194" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>1850</v>
       </c>
@@ -9539,16 +9593,10 @@
         <v>3</v>
       </c>
       <c r="BJ9">
+        <v>0.02</v>
+      </c>
+      <c r="BK9">
         <v>3</v>
-      </c>
-      <c r="BK9">
-        <v>0.02</v>
-      </c>
-      <c r="BL9">
-        <v>3</v>
-      </c>
-      <c r="BM9">
-        <v>0.02</v>
       </c>
       <c r="BN9">
         <v>0.5</v>
@@ -9709,32 +9757,32 @@
       <c r="DU9">
         <v>1</v>
       </c>
-      <c r="FD9">
+      <c r="FF9">
         <v>34871</v>
       </c>
-      <c r="FE9">
+      <c r="FG9">
         <v>47538</v>
       </c>
-      <c r="FF9">
+      <c r="FH9">
         <v>18.36</v>
       </c>
-      <c r="FG9">
+      <c r="FI9">
         <v>22.99</v>
       </c>
-      <c r="GG9" t="s">
+      <c r="GI9" t="s">
         <v>417</v>
       </c>
-      <c r="GH9" t="s">
+      <c r="GJ9" t="s">
         <v>6</v>
       </c>
-      <c r="GI9" t="s">
+      <c r="GK9" t="s">
         <v>621</v>
       </c>
-      <c r="GJ9" t="s">
+      <c r="GL9" t="s">
         <v>1878</v>
       </c>
     </row>
-    <row r="10" spans="1:192" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:194" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>1851</v>
       </c>
@@ -10068,41 +10116,41 @@
       <c r="EK10">
         <v>92307</v>
       </c>
-      <c r="EP10">
+      <c r="ER10">
         <v>30988</v>
       </c>
-      <c r="EQ10">
+      <c r="ES10">
         <v>43766</v>
       </c>
-      <c r="ER10">
+      <c r="ET10">
         <v>16.149999999999999</v>
       </c>
-      <c r="ES10">
+      <c r="EU10">
         <v>22.92</v>
       </c>
-      <c r="ET10">
+      <c r="EV10">
         <v>31493</v>
       </c>
-      <c r="EU10">
+      <c r="EW10">
         <v>44712</v>
       </c>
-      <c r="FT10">
+      <c r="FV10">
         <v>9.25</v>
       </c>
-      <c r="FU10">
+      <c r="FW10">
         <v>15</v>
       </c>
-      <c r="GH10" t="s">
+      <c r="GJ10" t="s">
         <v>7</v>
       </c>
-      <c r="GI10" t="s">
+      <c r="GK10" t="s">
         <v>1001</v>
       </c>
-      <c r="GJ10" t="s">
+      <c r="GL10" t="s">
         <v>1877</v>
       </c>
     </row>
-    <row r="11" spans="1:192" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:194" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>1852</v>
       </c>
@@ -10380,35 +10428,35 @@
       <c r="EC11">
         <v>41295.879999999997</v>
       </c>
-      <c r="EZ11">
+      <c r="FB11">
         <v>47387</v>
       </c>
-      <c r="FA11">
+      <c r="FC11">
         <v>47387</v>
       </c>
-      <c r="FN11">
+      <c r="FP11">
         <v>49173</v>
       </c>
-      <c r="FO11">
+      <c r="FQ11">
         <v>49173</v>
       </c>
-      <c r="FT11">
+      <c r="FV11">
         <v>9.1</v>
       </c>
-      <c r="FU11">
+      <c r="FW11">
         <v>9.1</v>
       </c>
-      <c r="GH11" t="s">
+      <c r="GJ11" t="s">
         <v>8</v>
       </c>
-      <c r="GI11" t="s">
+      <c r="GK11" t="s">
         <v>1002</v>
       </c>
-      <c r="GJ11" t="s">
+      <c r="GL11" t="s">
         <v>523</v>
       </c>
     </row>
-    <row r="12" spans="1:192" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:194" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>1261</v>
       </c>
@@ -10766,47 +10814,47 @@
       <c r="EM12">
         <v>30.28</v>
       </c>
-      <c r="ER12">
+      <c r="ET12">
         <v>19.239999999999998</v>
       </c>
-      <c r="ES12">
+      <c r="EU12">
         <v>19.239999999999998</v>
       </c>
-      <c r="EV12">
+      <c r="EX12">
         <v>25.98</v>
       </c>
-      <c r="EW12">
+      <c r="EY12">
         <v>25.98</v>
       </c>
-      <c r="FF12">
+      <c r="FH12">
         <v>16.09</v>
       </c>
-      <c r="FG12">
+      <c r="FI12">
         <v>18.690000000000001</v>
       </c>
-      <c r="FP12">
+      <c r="FR12">
         <v>103360.68</v>
       </c>
-      <c r="FQ12">
+      <c r="FS12">
         <v>103360.68</v>
       </c>
-      <c r="FR12">
+      <c r="FT12">
         <v>112200</v>
       </c>
-      <c r="FS12">
+      <c r="FU12">
         <v>112200</v>
       </c>
-      <c r="GH12" t="s">
+      <c r="GJ12" t="s">
         <v>1868</v>
       </c>
-      <c r="GI12" t="s">
+      <c r="GK12" t="s">
         <v>1003</v>
       </c>
-      <c r="GJ12" t="s">
+      <c r="GL12" t="s">
         <v>524</v>
       </c>
     </row>
-    <row r="13" spans="1:192" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:194" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>1853</v>
       </c>
@@ -10856,23 +10904,23 @@
         <v>1</v>
       </c>
       <c r="DL13"/>
-      <c r="FT13">
+      <c r="FV13">
         <v>8</v>
       </c>
-      <c r="FU13">
+      <c r="FW13">
         <v>8</v>
       </c>
-      <c r="GH13" t="s">
+      <c r="GJ13" t="s">
         <v>10</v>
       </c>
-      <c r="GI13" t="s">
+      <c r="GK13" t="s">
         <v>1004</v>
       </c>
-      <c r="GJ13" t="s">
+      <c r="GL13" t="s">
         <v>526</v>
       </c>
     </row>
-    <row r="14" spans="1:192" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:194" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>1845</v>
       </c>
@@ -11157,17 +11205,17 @@
       <c r="DS14">
         <v>12</v>
       </c>
-      <c r="GH14" t="s">
+      <c r="GJ14" t="s">
         <v>11</v>
       </c>
-      <c r="GI14" t="s">
+      <c r="GK14" t="s">
         <v>1005</v>
       </c>
-      <c r="GJ14" t="s">
+      <c r="GL14" t="s">
         <v>525</v>
       </c>
     </row>
-    <row r="15" spans="1:192" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:194" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>1638</v>
       </c>
@@ -11459,17 +11507,17 @@
       <c r="DQ15">
         <v>12</v>
       </c>
-      <c r="GH15" t="s">
+      <c r="GJ15" t="s">
         <v>12</v>
       </c>
-      <c r="GI15" t="s">
+      <c r="GK15" t="s">
         <v>1000</v>
       </c>
-      <c r="GJ15" t="s">
+      <c r="GL15" t="s">
         <v>554</v>
       </c>
     </row>
-    <row r="16" spans="1:192" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:194" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>1854</v>
       </c>
@@ -11797,89 +11845,89 @@
       <c r="EO16">
         <v>126162</v>
       </c>
-      <c r="EP16">
+      <c r="ER16">
         <v>29229</v>
       </c>
-      <c r="EQ16">
+      <c r="ES16">
         <v>52852</v>
       </c>
-      <c r="ER16">
+      <c r="ET16">
         <v>16.059999999999999</v>
       </c>
-      <c r="ES16">
+      <c r="EU16">
         <v>29.04</v>
       </c>
-      <c r="ET16">
+      <c r="EV16">
         <v>34634</v>
       </c>
-      <c r="EU16">
+      <c r="EW16">
         <v>62662</v>
       </c>
-      <c r="EX16">
+      <c r="EZ16">
         <v>38456</v>
       </c>
-      <c r="EY16">
+      <c r="FA16">
         <v>69560</v>
       </c>
-      <c r="EZ16">
+      <c r="FB16">
         <v>56256</v>
       </c>
-      <c r="FA16">
+      <c r="FC16">
         <v>101701</v>
       </c>
-      <c r="FB16">
+      <c r="FD16">
         <v>16.03</v>
       </c>
-      <c r="FC16">
+      <c r="FE16">
         <v>28.98</v>
       </c>
-      <c r="FD16">
+      <c r="FF16">
         <v>33560</v>
       </c>
-      <c r="FE16">
+      <c r="FG16">
         <v>60678</v>
       </c>
-      <c r="FF16">
+      <c r="FH16">
         <v>18.440000000000001</v>
       </c>
-      <c r="FG16">
+      <c r="FI16">
         <v>33.340000000000003</v>
       </c>
-      <c r="FH16">
+      <c r="FJ16">
         <v>38201</v>
       </c>
-      <c r="FI16">
+      <c r="FK16">
         <v>69105</v>
       </c>
-      <c r="FJ16">
+      <c r="FL16">
         <v>56256</v>
       </c>
-      <c r="FK16">
+      <c r="FM16">
         <v>101701</v>
       </c>
-      <c r="FP16">
+      <c r="FR16">
         <v>107000</v>
       </c>
-      <c r="FQ16">
+      <c r="FS16">
         <v>107000</v>
       </c>
-      <c r="FR16">
+      <c r="FT16">
         <v>125000</v>
       </c>
-      <c r="FS16">
+      <c r="FU16">
         <v>125000</v>
       </c>
-      <c r="GH16" t="s">
+      <c r="GJ16" t="s">
         <v>13</v>
       </c>
-      <c r="GI16" t="s">
+      <c r="GK16" t="s">
         <v>1006</v>
       </c>
-      <c r="GJ16" t="s">
+      <c r="GL16" t="s">
         <v>1061</v>
       </c>
     </row>
-    <row r="17" spans="1:192" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:194" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>1855</v>
       </c>
@@ -12255,41 +12303,41 @@
       <c r="EG17">
         <v>80000</v>
       </c>
-      <c r="FF17">
+      <c r="FH17">
         <v>15</v>
       </c>
-      <c r="FG17">
+      <c r="FI17">
         <v>22</v>
       </c>
-      <c r="FH17">
+      <c r="FJ17">
         <v>38000</v>
       </c>
-      <c r="FI17">
+      <c r="FK17">
         <v>50000</v>
       </c>
-      <c r="FL17">
+      <c r="FN17">
         <v>40000</v>
       </c>
-      <c r="FM17">
+      <c r="FO17">
         <v>58000</v>
       </c>
-      <c r="FT17">
+      <c r="FV17">
         <v>8.75</v>
       </c>
-      <c r="FU17">
+      <c r="FW17">
         <v>10.1</v>
       </c>
-      <c r="GH17" t="s">
+      <c r="GJ17" t="s">
         <v>14</v>
       </c>
-      <c r="GI17" t="s">
+      <c r="GK17" t="s">
         <v>1007</v>
       </c>
-      <c r="GJ17" t="s">
+      <c r="GL17" t="s">
         <v>556</v>
       </c>
     </row>
-    <row r="18" spans="1:192" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:194" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>1856</v>
       </c>
@@ -12698,77 +12746,77 @@
       <c r="EO18">
         <v>104642</v>
       </c>
-      <c r="EP18">
+      <c r="ER18">
         <v>32985</v>
       </c>
-      <c r="EQ18">
+      <c r="ES18">
         <v>44203</v>
       </c>
-      <c r="ER18">
+      <c r="ET18">
         <v>13.62</v>
       </c>
-      <c r="ES18">
+      <c r="EU18">
         <v>15.77</v>
       </c>
-      <c r="ET18">
+      <c r="EV18">
         <v>38184</v>
       </c>
-      <c r="EU18">
+      <c r="EW18">
         <v>51171</v>
       </c>
-      <c r="EX18">
+      <c r="EZ18">
         <v>51171</v>
       </c>
-      <c r="EY18">
+      <c r="FA18">
         <v>72002</v>
       </c>
-      <c r="FB18">
+      <c r="FD18">
         <v>19.899999999999999</v>
       </c>
-      <c r="FC18">
+      <c r="FE18">
         <v>19.899999999999999</v>
       </c>
-      <c r="FD18">
+      <c r="FF18">
         <v>36366</v>
       </c>
-      <c r="FE18">
+      <c r="FG18">
         <v>48734</v>
       </c>
-      <c r="FF18">
+      <c r="FH18">
         <v>13.62</v>
       </c>
-      <c r="FG18">
+      <c r="FI18">
         <v>15.77</v>
       </c>
-      <c r="FJ18">
+      <c r="FL18">
         <v>68573</v>
       </c>
-      <c r="FK18">
+      <c r="FM18">
         <v>91895</v>
       </c>
-      <c r="FP18">
+      <c r="FR18">
         <v>86089</v>
       </c>
-      <c r="FQ18">
+      <c r="FS18">
         <v>115368</v>
       </c>
-      <c r="FT18">
+      <c r="FV18">
         <v>8.75</v>
       </c>
-      <c r="FU18">
+      <c r="FW18">
         <v>9.5500000000000007</v>
       </c>
-      <c r="GH18" t="s">
+      <c r="GJ18" t="s">
         <v>15</v>
       </c>
-      <c r="GI18" t="s">
+      <c r="GK18" t="s">
         <v>1008</v>
       </c>
-      <c r="GJ18" t="s">
+      <c r="GL18" t="s">
         <v>557</v>
       </c>
     </row>
-    <row r="19" spans="1:192" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:194" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>1717</v>
       </c>
@@ -13004,35 +13052,35 @@
       <c r="EE19">
         <v>26.1</v>
       </c>
-      <c r="EV19">
+      <c r="EX19">
         <v>12</v>
       </c>
-      <c r="EW19">
+      <c r="EY19">
         <v>28.04</v>
       </c>
-      <c r="FF19">
+      <c r="FH19">
         <v>15</v>
       </c>
-      <c r="FG19">
+      <c r="FI19">
         <v>15</v>
       </c>
-      <c r="FT19">
+      <c r="FV19">
         <v>9</v>
       </c>
-      <c r="FU19">
+      <c r="FW19">
         <v>9</v>
       </c>
-      <c r="GH19" t="s">
+      <c r="GJ19" t="s">
         <v>17</v>
       </c>
-      <c r="GI19" t="s">
+      <c r="GK19" t="s">
         <v>1009</v>
       </c>
-      <c r="GJ19" t="s">
+      <c r="GL19" t="s">
         <v>575</v>
       </c>
     </row>
-    <row r="20" spans="1:192" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:194" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>1857</v>
       </c>
@@ -13381,71 +13429,71 @@
       <c r="EK20">
         <v>102602</v>
       </c>
-      <c r="EP20">
+      <c r="ER20">
         <v>30306</v>
       </c>
-      <c r="EQ20">
+      <c r="ES20">
         <v>51215</v>
       </c>
-      <c r="ER20">
+      <c r="ET20">
         <v>15.87</v>
       </c>
-      <c r="ES20">
+      <c r="EU20">
         <v>26.82</v>
       </c>
-      <c r="ET20">
+      <c r="EV20">
         <v>40276</v>
       </c>
-      <c r="EU20">
+      <c r="EW20">
         <v>58922</v>
       </c>
-      <c r="FB20">
+      <c r="FD20">
         <v>17.489999999999998</v>
       </c>
-      <c r="FC20">
+      <c r="FE20">
         <v>17.489999999999998</v>
       </c>
-      <c r="FD20">
+      <c r="FF20">
         <v>31728</v>
       </c>
-      <c r="FE20">
+      <c r="FG20">
         <v>53613</v>
       </c>
-      <c r="FF20">
+      <c r="FH20">
         <v>15.13</v>
       </c>
-      <c r="FG20">
+      <c r="FI20">
         <v>25.56</v>
       </c>
-      <c r="FH20">
+      <c r="FJ20">
         <v>34867</v>
       </c>
-      <c r="FI20">
+      <c r="FK20">
         <v>58992</v>
       </c>
-      <c r="FL20">
+      <c r="FN20">
         <v>50693</v>
       </c>
-      <c r="FM20">
+      <c r="FO20">
         <v>85668</v>
       </c>
-      <c r="FT20">
+      <c r="FV20">
         <v>8.75</v>
       </c>
-      <c r="FU20">
+      <c r="FW20">
         <v>12.5</v>
       </c>
-      <c r="GH20" t="s">
+      <c r="GJ20" t="s">
         <v>16</v>
       </c>
-      <c r="GI20" t="s">
+      <c r="GK20" t="s">
         <v>1010</v>
       </c>
-      <c r="GJ20" t="s">
+      <c r="GL20" t="s">
         <v>577</v>
       </c>
     </row>
-    <row r="21" spans="1:192" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:194" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>1858</v>
       </c>
@@ -13812,41 +13860,41 @@
       <c r="EM21">
         <v>32.76</v>
       </c>
-      <c r="ER21">
+      <c r="ET21">
         <v>19.02</v>
       </c>
-      <c r="ES21">
+      <c r="EU21">
         <v>27.16</v>
       </c>
-      <c r="EV21">
+      <c r="EX21">
         <v>21.83</v>
       </c>
-      <c r="EW21">
+      <c r="EY21">
         <v>33.090000000000003</v>
       </c>
-      <c r="FF21">
+      <c r="FH21">
         <v>16.32</v>
       </c>
-      <c r="FG21">
+      <c r="FI21">
         <v>16.32</v>
       </c>
-      <c r="FT21">
+      <c r="FV21">
         <v>8.75</v>
       </c>
-      <c r="FU21">
+      <c r="FW21">
         <v>10.72</v>
       </c>
-      <c r="GH21" t="s">
+      <c r="GJ21" t="s">
         <v>18</v>
       </c>
-      <c r="GI21" t="s">
+      <c r="GK21" t="s">
         <v>1011</v>
       </c>
-      <c r="GJ21" t="s">
+      <c r="GL21" t="s">
         <v>1133</v>
       </c>
     </row>
-    <row r="22" spans="1:192" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:194" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>1859</v>
       </c>
@@ -14138,17 +14186,17 @@
       <c r="DV22">
         <v>5</v>
       </c>
-      <c r="GH22" t="s">
+      <c r="GJ22" t="s">
         <v>19</v>
       </c>
-      <c r="GI22" t="s">
+      <c r="GK22" t="s">
         <v>1098</v>
       </c>
-      <c r="GJ22" t="s">
+      <c r="GL22" t="s">
         <v>579</v>
       </c>
     </row>
-    <row r="23" spans="1:192" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:194" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>1389</v>
       </c>
@@ -14419,35 +14467,35 @@
       <c r="EE23">
         <v>49.09</v>
       </c>
-      <c r="ER23">
+      <c r="ET23">
         <v>17.45</v>
       </c>
-      <c r="ES23">
+      <c r="EU23">
         <v>27.52</v>
       </c>
-      <c r="EZ23">
+      <c r="FB23">
         <v>21.48</v>
       </c>
-      <c r="FA23">
+      <c r="FC23">
         <v>33.99</v>
       </c>
-      <c r="FF23">
+      <c r="FH23">
         <v>17.45</v>
       </c>
-      <c r="FG23">
+      <c r="FI23">
         <v>27.52</v>
       </c>
-      <c r="GH23" t="s">
+      <c r="GJ23" t="s">
         <v>20</v>
       </c>
-      <c r="GI23" t="s">
+      <c r="GK23" t="s">
         <v>1012</v>
       </c>
-      <c r="GJ23" t="s">
+      <c r="GL23" t="s">
         <v>580</v>
       </c>
     </row>
-    <row r="24" spans="1:192" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:194" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>1860</v>
       </c>
@@ -14769,74 +14817,74 @@
       <c r="EK24">
         <v>68700</v>
       </c>
-      <c r="EP24">
+      <c r="ER24">
         <v>25700</v>
       </c>
-      <c r="EQ24">
+      <c r="ES24">
         <v>35300</v>
       </c>
-      <c r="ER24">
+      <c r="ET24">
         <v>14.09</v>
       </c>
-      <c r="ES24">
+      <c r="EU24">
         <v>21.49</v>
       </c>
-      <c r="ET24">
+      <c r="EV24">
         <v>30300</v>
       </c>
-      <c r="EU24">
+      <c r="EW24">
         <v>30800</v>
       </c>
-      <c r="EZ24">
+      <c r="FB24">
         <v>34850</v>
       </c>
-      <c r="FA24">
+      <c r="FC24">
         <v>49900</v>
       </c>
-      <c r="FB24">
+      <c r="FD24">
         <v>19</v>
       </c>
-      <c r="FC24">
+      <c r="FE24">
         <v>21.1</v>
       </c>
-      <c r="FF24">
+      <c r="FH24">
         <v>14.95</v>
       </c>
-      <c r="FL24">
+      <c r="FN24">
         <v>27200</v>
       </c>
-      <c r="FM24">
+      <c r="FO24">
         <v>49900</v>
       </c>
-      <c r="FN24">
+      <c r="FP24">
         <v>34850</v>
       </c>
-      <c r="FO24">
+      <c r="FQ24">
         <v>60000</v>
       </c>
-      <c r="FR24">
+      <c r="FT24">
         <v>95000</v>
       </c>
-      <c r="FS24">
+      <c r="FU24">
         <v>120000</v>
       </c>
-      <c r="FT24">
+      <c r="FV24">
         <v>8.93</v>
       </c>
-      <c r="FU24">
+      <c r="FW24">
         <v>9.36</v>
       </c>
-      <c r="GH24" t="s">
+      <c r="GJ24" t="s">
         <v>21</v>
       </c>
-      <c r="GI24" t="s">
+      <c r="GK24" t="s">
         <v>1013</v>
       </c>
-      <c r="GJ24" t="s">
+      <c r="GL24" t="s">
         <v>581</v>
       </c>
     </row>
-    <row r="25" spans="1:192" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:194" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>1861</v>
       </c>
@@ -15150,47 +15198,47 @@
       <c r="EO25">
         <v>84000</v>
       </c>
-      <c r="EP25">
+      <c r="ER25">
         <v>17000</v>
       </c>
-      <c r="EQ25">
+      <c r="ES25">
         <v>34000</v>
       </c>
-      <c r="ER25">
+      <c r="ET25">
         <v>14.3</v>
       </c>
-      <c r="ES25">
+      <c r="EU25">
         <v>18.89</v>
       </c>
-      <c r="EZ25">
+      <c r="FB25">
         <v>50000</v>
       </c>
-      <c r="FA25">
+      <c r="FC25">
         <v>50000</v>
       </c>
-      <c r="FF25">
+      <c r="FH25">
         <v>15.66</v>
       </c>
-      <c r="FG25">
+      <c r="FI25">
         <v>17.07</v>
       </c>
-      <c r="FN25">
+      <c r="FP25">
         <v>30000</v>
       </c>
-      <c r="FO25">
+      <c r="FQ25">
         <v>63000</v>
       </c>
-      <c r="FR25">
+      <c r="FT25">
         <v>115000</v>
       </c>
-      <c r="GI25" t="s">
+      <c r="GK25" t="s">
         <v>1323</v>
       </c>
-      <c r="GJ25" t="s">
+      <c r="GL25" t="s">
         <v>582</v>
       </c>
     </row>
-    <row r="26" spans="1:192" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:194" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>1488</v>
       </c>
@@ -15482,68 +15530,68 @@
       <c r="EK26">
         <v>91800</v>
       </c>
-      <c r="EP26">
+      <c r="ER26">
         <v>22276</v>
       </c>
-      <c r="EQ26">
+      <c r="ES26">
         <v>35700</v>
       </c>
-      <c r="ER26">
+      <c r="ET26">
         <v>12.24</v>
       </c>
-      <c r="ES26">
+      <c r="EU26">
         <v>20.399999999999999</v>
       </c>
-      <c r="ET26">
+      <c r="EV26">
         <v>29702</v>
       </c>
-      <c r="EU26">
+      <c r="EW26">
         <v>40800</v>
       </c>
-      <c r="EV26">
+      <c r="EX26">
         <v>16.32</v>
       </c>
-      <c r="EW26">
+      <c r="EY26">
         <v>22.44</v>
       </c>
-      <c r="FD26">
+      <c r="FF26">
         <v>27580</v>
       </c>
-      <c r="FE26">
+      <c r="FG26">
         <v>35700</v>
       </c>
-      <c r="FF26">
+      <c r="FH26">
         <v>13.26</v>
       </c>
-      <c r="FG26">
+      <c r="FI26">
         <v>18.36</v>
       </c>
-      <c r="FH26">
+      <c r="FJ26">
         <v>33435</v>
       </c>
-      <c r="FI26">
+      <c r="FK26">
         <v>45900</v>
       </c>
-      <c r="FJ26">
+      <c r="FL26">
         <v>41336</v>
       </c>
-      <c r="FK26">
+      <c r="FM26">
         <v>51000</v>
       </c>
-      <c r="FT26">
+      <c r="FV26">
         <v>8.75</v>
       </c>
-      <c r="FU26">
+      <c r="FW26">
         <v>8.75</v>
       </c>
-      <c r="GI26" t="s">
+      <c r="GK26" t="s">
         <v>1014</v>
       </c>
-      <c r="GJ26" t="s">
+      <c r="GL26" t="s">
         <v>583</v>
       </c>
     </row>
-    <row r="27" spans="1:192" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:194" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>1489</v>
       </c>
@@ -15830,62 +15878,62 @@
       <c r="EK27">
         <v>67384</v>
       </c>
-      <c r="ER27">
+      <c r="ET27">
         <v>13</v>
       </c>
-      <c r="ES27">
+      <c r="EU27">
         <v>13</v>
       </c>
-      <c r="ET27">
+      <c r="EV27">
         <v>45350</v>
       </c>
-      <c r="EU27">
+      <c r="EW27">
         <v>45350</v>
       </c>
-      <c r="EX27">
+      <c r="EZ27">
         <v>47600</v>
       </c>
-      <c r="EY27">
+      <c r="FA27">
         <v>47600</v>
       </c>
-      <c r="FD27">
+      <c r="FF27">
         <v>34000</v>
       </c>
-      <c r="FE27">
+      <c r="FG27">
         <v>34000</v>
       </c>
-      <c r="FF27">
+      <c r="FH27">
         <v>14</v>
       </c>
-      <c r="FH27">
+      <c r="FJ27">
         <v>39500</v>
       </c>
-      <c r="FI27">
+      <c r="FK27">
         <v>39500</v>
       </c>
-      <c r="FP27">
+      <c r="FR27">
         <v>107000</v>
       </c>
-      <c r="FQ27">
+      <c r="FS27">
         <v>107000</v>
       </c>
-      <c r="FR27">
+      <c r="FT27">
         <v>155000</v>
       </c>
-      <c r="FT27">
+      <c r="FV27">
         <v>12</v>
       </c>
-      <c r="FU27">
+      <c r="FW27">
         <v>12</v>
       </c>
-      <c r="GI27" t="s">
+      <c r="GK27" t="s">
         <v>1015</v>
       </c>
-      <c r="GJ27" t="s">
+      <c r="GL27" t="s">
         <v>585</v>
       </c>
     </row>
-    <row r="28" spans="1:192" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:194" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>1862</v>
       </c>
@@ -16117,14 +16165,14 @@
       <c r="DW28">
         <v>0</v>
       </c>
-      <c r="GI28" t="s">
+      <c r="GK28" t="s">
         <v>1016</v>
       </c>
-      <c r="GJ28" t="s">
+      <c r="GL28" t="s">
         <v>637</v>
       </c>
     </row>
-    <row r="29" spans="1:192" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:194" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>1863</v>
       </c>
@@ -16440,71 +16488,71 @@
       <c r="EO29">
         <v>94850</v>
       </c>
-      <c r="EP29">
+      <c r="ER29">
         <v>30336</v>
       </c>
-      <c r="EQ29">
+      <c r="ES29">
         <v>48497</v>
       </c>
-      <c r="ER29">
+      <c r="ET29">
         <v>16.670000000000002</v>
       </c>
-      <c r="ES29">
+      <c r="EU29">
         <v>26.65</v>
       </c>
-      <c r="ET29">
+      <c r="EV29">
         <v>35486</v>
       </c>
-      <c r="EU29">
+      <c r="EW29">
         <v>54655</v>
       </c>
-      <c r="FD29">
+      <c r="FF29">
         <v>33370</v>
       </c>
-      <c r="FE29">
+      <c r="FG29">
         <v>51762</v>
       </c>
-      <c r="FF29">
+      <c r="FH29">
         <v>18.34</v>
       </c>
-      <c r="FG29">
+      <c r="FI29">
         <v>28.44</v>
       </c>
-      <c r="FJ29">
+      <c r="FL29">
         <v>45669</v>
       </c>
-      <c r="FK29">
+      <c r="FM29">
         <v>65743</v>
       </c>
-      <c r="FN29">
+      <c r="FP29">
         <v>52670</v>
       </c>
-      <c r="FO29">
+      <c r="FQ29">
         <v>79323</v>
       </c>
-      <c r="FP29">
+      <c r="FR29">
         <v>83000</v>
       </c>
-      <c r="FQ29">
+      <c r="FS29">
         <v>110682</v>
       </c>
-      <c r="FR29">
+      <c r="FT29">
         <v>171532</v>
       </c>
-      <c r="FT29">
+      <c r="FV29">
         <v>8.75</v>
       </c>
-      <c r="FU29">
+      <c r="FW29">
         <v>8.75</v>
       </c>
-      <c r="GI29" t="s">
+      <c r="GK29" t="s">
         <v>1243</v>
       </c>
-      <c r="GJ29" t="s">
+      <c r="GL29" t="s">
         <v>639</v>
       </c>
     </row>
-    <row r="30" spans="1:192" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:194" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>1864</v>
       </c>
@@ -16824,32 +16872,32 @@
       <c r="EK30">
         <v>75435</v>
       </c>
-      <c r="EP30">
+      <c r="ER30">
         <v>33386</v>
       </c>
-      <c r="EQ30">
+      <c r="ES30">
         <v>52284</v>
       </c>
-      <c r="ER30">
+      <c r="ET30">
         <v>15.23</v>
       </c>
-      <c r="ES30">
+      <c r="EU30">
         <v>20.61</v>
       </c>
-      <c r="FT30">
+      <c r="FV30">
         <v>9.6</v>
       </c>
-      <c r="FU30">
+      <c r="FW30">
         <v>10.11</v>
       </c>
-      <c r="GI30" t="s">
+      <c r="GK30" t="s">
         <v>1017</v>
       </c>
-      <c r="GJ30" t="s">
+      <c r="GL30" t="s">
         <v>640</v>
       </c>
     </row>
-    <row r="31" spans="1:192" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:194" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>1865</v>
       </c>
@@ -17198,388 +17246,388 @@
       <c r="EE31">
         <v>25.89</v>
       </c>
-      <c r="ER31">
+      <c r="ET31">
         <v>13.99</v>
       </c>
-      <c r="ES31">
+      <c r="EU31">
         <v>20.34</v>
       </c>
-      <c r="EV31">
+      <c r="EX31">
         <v>13.32</v>
       </c>
-      <c r="EW31">
+      <c r="EY31">
         <v>17.309999999999999</v>
       </c>
-      <c r="GI31" t="s">
+      <c r="GK31" t="s">
         <v>1396</v>
       </c>
-      <c r="GJ31" t="s">
+      <c r="GL31" t="s">
         <v>642</v>
       </c>
     </row>
-    <row r="32" spans="1:192" x14ac:dyDescent="0.35">
-      <c r="GI32" t="s">
+    <row r="32" spans="1:194" x14ac:dyDescent="0.35">
+      <c r="GK32" t="s">
         <v>1018</v>
       </c>
-      <c r="GJ32" t="s">
+      <c r="GL32" t="s">
         <v>643</v>
       </c>
     </row>
-    <row r="33" spans="191:192" x14ac:dyDescent="0.35">
-      <c r="GI33" t="s">
+    <row r="33" spans="193:194" x14ac:dyDescent="0.35">
+      <c r="GK33" t="s">
         <v>1019</v>
       </c>
-      <c r="GJ33" t="s">
+      <c r="GL33" t="s">
         <v>645</v>
       </c>
     </row>
-    <row r="34" spans="191:192" x14ac:dyDescent="0.35">
-      <c r="GI34" t="s">
+    <row r="34" spans="193:194" x14ac:dyDescent="0.35">
+      <c r="GK34" t="s">
         <v>1020</v>
       </c>
-      <c r="GJ34" t="s">
+      <c r="GL34" t="s">
         <v>646</v>
       </c>
     </row>
-    <row r="35" spans="191:192" x14ac:dyDescent="0.35">
-      <c r="GI35" t="s">
+    <row r="35" spans="193:194" x14ac:dyDescent="0.35">
+      <c r="GK35" t="s">
         <v>1021</v>
       </c>
-      <c r="GJ35" t="s">
+      <c r="GL35" t="s">
         <v>648</v>
       </c>
     </row>
-    <row r="36" spans="191:192" x14ac:dyDescent="0.35">
-      <c r="GI36" t="s">
+    <row r="36" spans="193:194" x14ac:dyDescent="0.35">
+      <c r="GK36" t="s">
         <v>1022</v>
       </c>
-      <c r="GJ36" t="s">
+      <c r="GL36" t="s">
         <v>649</v>
       </c>
     </row>
-    <row r="37" spans="191:192" x14ac:dyDescent="0.35">
-      <c r="GI37" t="s">
+    <row r="37" spans="193:194" x14ac:dyDescent="0.35">
+      <c r="GK37" t="s">
         <v>1023</v>
       </c>
-      <c r="GJ37" t="s">
+      <c r="GL37" t="s">
         <v>659</v>
       </c>
     </row>
-    <row r="38" spans="191:192" x14ac:dyDescent="0.35">
-      <c r="GI38" t="s">
+    <row r="38" spans="193:194" x14ac:dyDescent="0.35">
+      <c r="GK38" t="s">
         <v>1024</v>
       </c>
-      <c r="GJ38" t="s">
+      <c r="GL38" t="s">
         <v>660</v>
       </c>
     </row>
-    <row r="39" spans="191:192" x14ac:dyDescent="0.35">
-      <c r="GI39" t="s">
+    <row r="39" spans="193:194" x14ac:dyDescent="0.35">
+      <c r="GK39" t="s">
         <v>1025</v>
       </c>
-      <c r="GJ39" t="s">
+      <c r="GL39" t="s">
         <v>560</v>
       </c>
     </row>
-    <row r="40" spans="191:192" x14ac:dyDescent="0.35">
-      <c r="GI40" t="s">
+    <row r="40" spans="193:194" x14ac:dyDescent="0.35">
+      <c r="GK40" t="s">
         <v>1026</v>
       </c>
-      <c r="GJ40" t="s">
+      <c r="GL40" t="s">
         <v>561</v>
       </c>
     </row>
-    <row r="41" spans="191:192" x14ac:dyDescent="0.35">
-      <c r="GI41" t="s">
+    <row r="41" spans="193:194" x14ac:dyDescent="0.35">
+      <c r="GK41" t="s">
         <v>1027</v>
       </c>
-      <c r="GJ41" t="s">
+      <c r="GL41" t="s">
         <v>662</v>
       </c>
     </row>
-    <row r="42" spans="191:192" x14ac:dyDescent="0.35">
-      <c r="GI42" t="s">
+    <row r="42" spans="193:194" x14ac:dyDescent="0.35">
+      <c r="GK42" t="s">
         <v>1028</v>
       </c>
-      <c r="GJ42" t="s">
+      <c r="GL42" t="s">
         <v>663</v>
       </c>
     </row>
-    <row r="43" spans="191:192" x14ac:dyDescent="0.35">
-      <c r="GI43" t="s">
+    <row r="43" spans="193:194" x14ac:dyDescent="0.35">
+      <c r="GK43" t="s">
         <v>510</v>
       </c>
-      <c r="GJ43" t="s">
+      <c r="GL43" t="s">
         <v>665</v>
       </c>
     </row>
-    <row r="44" spans="191:192" x14ac:dyDescent="0.35">
-      <c r="GI44" t="s">
+    <row r="44" spans="193:194" x14ac:dyDescent="0.35">
+      <c r="GK44" t="s">
         <v>1140</v>
       </c>
-      <c r="GJ44" t="s">
+      <c r="GL44" t="s">
         <v>666</v>
       </c>
     </row>
-    <row r="45" spans="191:192" x14ac:dyDescent="0.35">
-      <c r="GI45" t="s">
+    <row r="45" spans="193:194" x14ac:dyDescent="0.35">
+      <c r="GK45" t="s">
         <v>1141</v>
       </c>
-      <c r="GJ45" t="s">
+      <c r="GL45" t="s">
         <v>668</v>
       </c>
     </row>
-    <row r="46" spans="191:192" x14ac:dyDescent="0.35">
-      <c r="GI46" t="s">
+    <row r="46" spans="193:194" x14ac:dyDescent="0.35">
+      <c r="GK46" t="s">
         <v>1142</v>
       </c>
-      <c r="GJ46" t="s">
+      <c r="GL46" t="s">
         <v>669</v>
       </c>
     </row>
-    <row r="47" spans="191:192" x14ac:dyDescent="0.35">
-      <c r="GI47" t="s">
+    <row r="47" spans="193:194" x14ac:dyDescent="0.35">
+      <c r="GK47" t="s">
         <v>1143</v>
       </c>
-      <c r="GJ47" t="s">
+      <c r="GL47" t="s">
         <v>729</v>
       </c>
     </row>
-    <row r="48" spans="191:192" x14ac:dyDescent="0.35">
-      <c r="GI48" t="s">
+    <row r="48" spans="193:194" x14ac:dyDescent="0.35">
+      <c r="GK48" t="s">
         <v>1144</v>
       </c>
-      <c r="GJ48" t="s">
+      <c r="GL48" t="s">
         <v>730</v>
       </c>
     </row>
-    <row r="49" spans="191:192" x14ac:dyDescent="0.35">
-      <c r="GI49" t="s">
+    <row r="49" spans="193:194" x14ac:dyDescent="0.35">
+      <c r="GK49" t="s">
         <v>1145</v>
       </c>
-      <c r="GJ49" t="s">
+      <c r="GL49" t="s">
         <v>872</v>
       </c>
     </row>
-    <row r="50" spans="191:192" x14ac:dyDescent="0.35">
-      <c r="GI50" t="s">
+    <row r="50" spans="193:194" x14ac:dyDescent="0.35">
+      <c r="GK50" t="s">
         <v>1146</v>
       </c>
-      <c r="GJ50" t="s">
+      <c r="GL50" t="s">
         <v>873</v>
       </c>
     </row>
-    <row r="51" spans="191:192" x14ac:dyDescent="0.35">
-      <c r="GI51" t="s">
+    <row r="51" spans="193:194" x14ac:dyDescent="0.35">
+      <c r="GK51" t="s">
         <v>1147</v>
       </c>
-      <c r="GJ51" t="s">
+      <c r="GL51" t="s">
         <v>887</v>
       </c>
     </row>
-    <row r="52" spans="191:192" x14ac:dyDescent="0.35">
-      <c r="GI52" t="s">
+    <row r="52" spans="193:194" x14ac:dyDescent="0.35">
+      <c r="GK52" t="s">
         <v>1148</v>
       </c>
-      <c r="GJ52" t="s">
+      <c r="GL52" t="s">
         <v>888</v>
       </c>
     </row>
-    <row r="53" spans="191:192" x14ac:dyDescent="0.35">
-      <c r="GI53" t="s">
+    <row r="53" spans="193:194" x14ac:dyDescent="0.35">
+      <c r="GK53" t="s">
         <v>1149</v>
       </c>
-      <c r="GJ53" t="s">
+      <c r="GL53" t="s">
         <v>597</v>
       </c>
     </row>
-    <row r="54" spans="191:192" x14ac:dyDescent="0.35">
-      <c r="GI54" t="s">
+    <row r="54" spans="193:194" x14ac:dyDescent="0.35">
+      <c r="GK54" t="s">
         <v>1150</v>
       </c>
-      <c r="GJ54" t="s">
+      <c r="GL54" t="s">
         <v>596</v>
       </c>
     </row>
-    <row r="55" spans="191:192" x14ac:dyDescent="0.35">
-      <c r="GI55" t="s">
+    <row r="55" spans="193:194" x14ac:dyDescent="0.35">
+      <c r="GK55" t="s">
         <v>1151</v>
       </c>
-      <c r="GJ55" t="s">
+      <c r="GL55" t="s">
         <v>598</v>
       </c>
     </row>
-    <row r="56" spans="191:192" x14ac:dyDescent="0.35">
-      <c r="GI56" t="s">
+    <row r="56" spans="193:194" x14ac:dyDescent="0.35">
+      <c r="GK56" t="s">
         <v>1152</v>
       </c>
-      <c r="GJ56" t="s">
+      <c r="GL56" t="s">
         <v>890</v>
       </c>
     </row>
-    <row r="57" spans="191:192" x14ac:dyDescent="0.35">
-      <c r="GI57" t="s">
+    <row r="57" spans="193:194" x14ac:dyDescent="0.35">
+      <c r="GK57" t="s">
         <v>1153</v>
       </c>
-      <c r="GJ57" t="s">
+      <c r="GL57" t="s">
         <v>894</v>
       </c>
     </row>
-    <row r="58" spans="191:192" x14ac:dyDescent="0.35">
-      <c r="GI58" t="s">
+    <row r="58" spans="193:194" x14ac:dyDescent="0.35">
+      <c r="GK58" t="s">
         <v>1154</v>
       </c>
-      <c r="GJ58" t="s">
+      <c r="GL58" t="s">
         <v>895</v>
       </c>
     </row>
-    <row r="59" spans="191:192" x14ac:dyDescent="0.35">
-      <c r="GI59" t="s">
+    <row r="59" spans="193:194" x14ac:dyDescent="0.35">
+      <c r="GK59" t="s">
         <v>1155</v>
       </c>
-      <c r="GJ59" t="s">
+      <c r="GL59" t="s">
         <v>601</v>
       </c>
     </row>
-    <row r="60" spans="191:192" x14ac:dyDescent="0.35">
-      <c r="GI60" t="s">
+    <row r="60" spans="193:194" x14ac:dyDescent="0.35">
+      <c r="GK60" t="s">
         <v>1156</v>
       </c>
-      <c r="GJ60" t="s">
+      <c r="GL60" t="s">
         <v>602</v>
       </c>
     </row>
-    <row r="61" spans="191:192" x14ac:dyDescent="0.35">
-      <c r="GI61" t="s">
+    <row r="61" spans="193:194" x14ac:dyDescent="0.35">
+      <c r="GK61" t="s">
         <v>1157</v>
       </c>
-      <c r="GJ61" t="s">
+      <c r="GL61" t="s">
         <v>943</v>
       </c>
     </row>
-    <row r="62" spans="191:192" x14ac:dyDescent="0.35">
-      <c r="GI62" t="s">
+    <row r="62" spans="193:194" x14ac:dyDescent="0.35">
+      <c r="GK62" t="s">
         <v>1158</v>
       </c>
-      <c r="GJ62" t="s">
+      <c r="GL62" t="s">
         <v>944</v>
       </c>
     </row>
-    <row r="63" spans="191:192" x14ac:dyDescent="0.35">
-      <c r="GI63" t="s">
+    <row r="63" spans="193:194" x14ac:dyDescent="0.35">
+      <c r="GK63" t="s">
         <v>1159</v>
       </c>
-      <c r="GJ63" t="s">
+      <c r="GL63" t="s">
         <v>609</v>
       </c>
     </row>
-    <row r="64" spans="191:192" x14ac:dyDescent="0.35">
-      <c r="GI64" t="s">
+    <row r="64" spans="193:194" x14ac:dyDescent="0.35">
+      <c r="GK64" t="s">
         <v>1160</v>
       </c>
-      <c r="GJ64" t="s">
+      <c r="GL64" t="s">
         <v>976</v>
       </c>
     </row>
-    <row r="65" spans="191:192" x14ac:dyDescent="0.35">
-      <c r="GI65" t="s">
+    <row r="65" spans="193:194" x14ac:dyDescent="0.35">
+      <c r="GK65" t="s">
         <v>1161</v>
       </c>
-      <c r="GJ65" t="s">
+      <c r="GL65" t="s">
         <v>981</v>
       </c>
     </row>
-    <row r="66" spans="191:192" x14ac:dyDescent="0.35">
-      <c r="GI66" t="s">
+    <row r="66" spans="193:194" x14ac:dyDescent="0.35">
+      <c r="GK66" t="s">
         <v>1162</v>
       </c>
-      <c r="GJ66" t="s">
+      <c r="GL66" t="s">
         <v>982</v>
       </c>
     </row>
-    <row r="67" spans="191:192" x14ac:dyDescent="0.35">
-      <c r="GI67" t="s">
+    <row r="67" spans="193:194" x14ac:dyDescent="0.35">
+      <c r="GK67" t="s">
         <v>1163</v>
       </c>
-      <c r="GJ67" t="s">
+      <c r="GL67" t="s">
         <v>610</v>
       </c>
     </row>
-    <row r="68" spans="191:192" x14ac:dyDescent="0.35">
-      <c r="GI68" t="s">
+    <row r="68" spans="193:194" x14ac:dyDescent="0.35">
+      <c r="GK68" t="s">
         <v>1164</v>
       </c>
-      <c r="GJ68" t="s">
+      <c r="GL68" t="s">
         <v>611</v>
       </c>
     </row>
-    <row r="69" spans="191:192" x14ac:dyDescent="0.35">
-      <c r="GI69" t="s">
+    <row r="69" spans="193:194" x14ac:dyDescent="0.35">
+      <c r="GK69" t="s">
         <v>1165</v>
       </c>
     </row>
-    <row r="70" spans="191:192" x14ac:dyDescent="0.35">
-      <c r="GI70" t="s">
+    <row r="70" spans="193:194" x14ac:dyDescent="0.35">
+      <c r="GK70" t="s">
         <v>1100</v>
       </c>
     </row>
-    <row r="71" spans="191:192" x14ac:dyDescent="0.35">
-      <c r="GI71" t="s">
+    <row r="71" spans="193:194" x14ac:dyDescent="0.35">
+      <c r="GK71" t="s">
         <v>1099</v>
       </c>
     </row>
-    <row r="72" spans="191:192" x14ac:dyDescent="0.35">
-      <c r="GI72" t="s">
+    <row r="72" spans="193:194" x14ac:dyDescent="0.35">
+      <c r="GK72" t="s">
         <v>1101</v>
       </c>
     </row>
-    <row r="73" spans="191:192" x14ac:dyDescent="0.35">
-      <c r="GI73" t="s">
+    <row r="73" spans="193:194" x14ac:dyDescent="0.35">
+      <c r="GK73" t="s">
         <v>1166</v>
       </c>
     </row>
-    <row r="74" spans="191:192" x14ac:dyDescent="0.35">
-      <c r="GI74" t="s">
+    <row r="74" spans="193:194" x14ac:dyDescent="0.35">
+      <c r="GK74" t="s">
         <v>1167</v>
       </c>
     </row>
-    <row r="75" spans="191:192" x14ac:dyDescent="0.35">
-      <c r="GI75" t="s">
+    <row r="75" spans="193:194" x14ac:dyDescent="0.35">
+      <c r="GK75" t="s">
         <v>1169</v>
       </c>
     </row>
-    <row r="76" spans="191:192" x14ac:dyDescent="0.35">
-      <c r="GI76" t="s">
+    <row r="76" spans="193:194" x14ac:dyDescent="0.35">
+      <c r="GK76" t="s">
         <v>1168</v>
       </c>
     </row>
-    <row r="77" spans="191:192" x14ac:dyDescent="0.35">
-      <c r="GI77" t="s">
+    <row r="77" spans="193:194" x14ac:dyDescent="0.35">
+      <c r="GK77" t="s">
         <v>1184</v>
       </c>
     </row>
-    <row r="78" spans="191:192" x14ac:dyDescent="0.35">
-      <c r="GI78" t="s">
+    <row r="78" spans="193:194" x14ac:dyDescent="0.35">
+      <c r="GK78" t="s">
         <v>1102</v>
       </c>
     </row>
-    <row r="79" spans="191:192" x14ac:dyDescent="0.35">
-      <c r="GI79" t="s">
+    <row r="79" spans="193:194" x14ac:dyDescent="0.35">
+      <c r="GK79" t="s">
         <v>1103</v>
       </c>
     </row>
-    <row r="80" spans="191:192" x14ac:dyDescent="0.35">
-      <c r="GI80" t="s">
+    <row r="80" spans="193:194" x14ac:dyDescent="0.35">
+      <c r="GK80" t="s">
         <v>1104</v>
       </c>
     </row>
-    <row r="81" spans="191:191" x14ac:dyDescent="0.35">
-      <c r="GI81" t="s">
+    <row r="81" spans="193:193" x14ac:dyDescent="0.35">
+      <c r="GK81" t="s">
         <v>1105</v>
       </c>
     </row>
-    <row r="82" spans="191:191" x14ac:dyDescent="0.35">
-      <c r="GI82" t="s">
+    <row r="82" spans="193:193" x14ac:dyDescent="0.35">
+      <c r="GK82" t="s">
         <v>1106</v>
       </c>
     </row>
@@ -17593,8 +17641,8 @@
   <dimension ref="A2:XFD32"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="ST1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="TR3" sqref="TR3"/>
+      <pane xSplit="1" topLeftCell="AM1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AR3" sqref="AR3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -40840,122 +40888,122 @@
   <sheetData>
     <row r="4" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C4" t="s">
-        <v>1894</v>
+        <v>1890</v>
       </c>
     </row>
     <row r="5" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C5" t="s">
-        <v>1895</v>
+        <v>1891</v>
       </c>
     </row>
     <row r="6" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C6" t="s">
-        <v>1896</v>
+        <v>1892</v>
       </c>
     </row>
     <row r="7" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C7" t="s">
-        <v>1897</v>
+        <v>1893</v>
       </c>
     </row>
     <row r="8" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C8" t="s">
-        <v>1898</v>
+        <v>1894</v>
       </c>
     </row>
     <row r="9" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C9" t="s">
-        <v>1899</v>
+        <v>1895</v>
       </c>
     </row>
     <row r="10" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C10" t="s">
-        <v>1900</v>
+        <v>1896</v>
       </c>
     </row>
     <row r="11" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C11" t="s">
-        <v>1901</v>
+        <v>1897</v>
       </c>
     </row>
     <row r="12" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C12" t="s">
-        <v>1902</v>
+        <v>1898</v>
       </c>
     </row>
     <row r="13" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C13" t="s">
-        <v>1903</v>
+        <v>1899</v>
       </c>
     </row>
     <row r="14" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C14" t="s">
-        <v>1904</v>
+        <v>1900</v>
       </c>
     </row>
     <row r="15" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C15" t="s">
-        <v>1905</v>
+        <v>1901</v>
       </c>
     </row>
     <row r="16" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C16" t="s">
-        <v>1906</v>
+        <v>1902</v>
       </c>
     </row>
     <row r="17" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C17" t="s">
-        <v>1907</v>
+        <v>1903</v>
       </c>
     </row>
     <row r="18" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C18" t="s">
-        <v>1908</v>
+        <v>1904</v>
       </c>
     </row>
     <row r="19" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C19" t="s">
-        <v>1909</v>
+        <v>1905</v>
       </c>
     </row>
     <row r="20" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C20" t="s">
-        <v>1910</v>
+        <v>1906</v>
       </c>
     </row>
     <row r="21" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C21" t="s">
-        <v>1911</v>
+        <v>1907</v>
       </c>
     </row>
     <row r="22" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C22" t="s">
-        <v>1912</v>
+        <v>1908</v>
       </c>
     </row>
     <row r="23" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C23" t="s">
-        <v>1913</v>
+        <v>1909</v>
       </c>
     </row>
     <row r="24" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C24" t="s">
-        <v>1914</v>
+        <v>1910</v>
       </c>
     </row>
     <row r="25" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C25" t="s">
-        <v>1915</v>
+        <v>1911</v>
       </c>
     </row>
     <row r="26" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C26" t="s">
-        <v>1916</v>
+        <v>1912</v>
       </c>
     </row>
     <row r="27" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C27" t="s">
-        <v>1917</v>
+        <v>1913</v>
       </c>
     </row>
     <row r="28" spans="3:3" x14ac:dyDescent="0.35">
@@ -40965,47 +41013,47 @@
     </row>
     <row r="29" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C29" t="s">
-        <v>1918</v>
+        <v>1914</v>
       </c>
     </row>
     <row r="30" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C30" t="s">
-        <v>1919</v>
+        <v>1915</v>
       </c>
     </row>
     <row r="31" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C31" t="s">
-        <v>1920</v>
+        <v>1916</v>
       </c>
     </row>
     <row r="32" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C32" t="s">
-        <v>1921</v>
+        <v>1917</v>
       </c>
     </row>
     <row r="33" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C33" t="s">
-        <v>1922</v>
+        <v>1918</v>
       </c>
     </row>
     <row r="34" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C34" t="s">
-        <v>1923</v>
+        <v>1919</v>
       </c>
     </row>
     <row r="35" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C35" t="s">
-        <v>1924</v>
+        <v>1920</v>
       </c>
     </row>
     <row r="36" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C36" t="s">
-        <v>1925</v>
+        <v>1921</v>
       </c>
     </row>
     <row r="37" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C37" t="s">
-        <v>1926</v>
+        <v>1922</v>
       </c>
     </row>
     <row r="38" spans="3:3" x14ac:dyDescent="0.35">
@@ -41015,27 +41063,27 @@
     </row>
     <row r="39" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C39" t="s">
-        <v>1927</v>
+        <v>1923</v>
       </c>
     </row>
     <row r="40" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C40" t="s">
-        <v>1928</v>
+        <v>1924</v>
       </c>
     </row>
     <row r="41" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C41" t="s">
-        <v>1929</v>
+        <v>1925</v>
       </c>
     </row>
     <row r="42" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C42" t="s">
-        <v>1930</v>
+        <v>1926</v>
       </c>
     </row>
     <row r="43" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C43" t="s">
-        <v>1931</v>
+        <v>1927</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
After adding conditional panel to Salary page
</commit_message>
<xml_diff>
--- a/SCLASurvey.xlsx
+++ b/SCLASurvey.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4188" uniqueCount="2039">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4188" uniqueCount="2066">
   <si>
     <t xml:space="preserve">Director </t>
   </si>
@@ -5683,21 +5683,6 @@
     <t>Annual Leave Days_Paid Holidays</t>
   </si>
   <si>
-    <t>Clerk/Library Clerk_Part Time_Max Salary</t>
-  </si>
-  <si>
-    <t>Sen. Clerk/ Sen. Library Clerk _Part Time_ Max Salary</t>
-  </si>
-  <si>
-    <t>Security Guard _Part Time_ Max Salary</t>
-  </si>
-  <si>
-    <t>Custodial Worker I_Part Time_Max Salary</t>
-  </si>
-  <si>
-    <t>Page_Part Time_Max Salary</t>
-  </si>
-  <si>
     <t>Books_Adult_Daily</t>
   </si>
   <si>
@@ -6143,6 +6128,102 @@
   </si>
   <si>
     <t>MaxSal_Librarian IV_PT</t>
+  </si>
+  <si>
+    <t>MinSal_Clerk_FT</t>
+  </si>
+  <si>
+    <t>MaxSal_Clerk_FT</t>
+  </si>
+  <si>
+    <t>MinSal_Clerk_PT</t>
+  </si>
+  <si>
+    <t>MaxSal_Clerk_PT</t>
+  </si>
+  <si>
+    <t>MinSal_Senior Clerk_FT</t>
+  </si>
+  <si>
+    <t>MaxSal_Senior Clerk_FT</t>
+  </si>
+  <si>
+    <t>MinSal_Senior Clerk_PT</t>
+  </si>
+  <si>
+    <t>MaxSal_Senior Clerk_PT</t>
+  </si>
+  <si>
+    <t>MinSal_Principal Clerk_FT</t>
+  </si>
+  <si>
+    <t>MaxSal_Principal Clerk_FT</t>
+  </si>
+  <si>
+    <t>MinSal_Circulation Supervisor_FT</t>
+  </si>
+  <si>
+    <t>MaxSal_Circulation Supervisor_FT</t>
+  </si>
+  <si>
+    <t>MinSal_Security Guard_PT</t>
+  </si>
+  <si>
+    <t>MaxSal_Security Guard_PT</t>
+  </si>
+  <si>
+    <t>MinSal_Custodial Worker I_FT</t>
+  </si>
+  <si>
+    <t>MaxSal_Custodial Worker I_FT</t>
+  </si>
+  <si>
+    <t>MinSal_Custodial Worker I_PT</t>
+  </si>
+  <si>
+    <t>MaxSal_Custodial Worker I_PT</t>
+  </si>
+  <si>
+    <t>MinSal_Custodial Worker II_FT</t>
+  </si>
+  <si>
+    <t>MaxSal_Custodial Worker II_FT</t>
+  </si>
+  <si>
+    <t>MinSal_Custodial Worker III_FT</t>
+  </si>
+  <si>
+    <t>MaxSal_Custodial Worker III_FT</t>
+  </si>
+  <si>
+    <t>MinSal_Head Custodian_FT</t>
+  </si>
+  <si>
+    <t>MaxSal_Head Custodian_FT</t>
+  </si>
+  <si>
+    <t>MinSal_Administrative Assistant_FT</t>
+  </si>
+  <si>
+    <t>MaxSal_Administrative Assistant_FT</t>
+  </si>
+  <si>
+    <t>MinSal_Assistant Director_FT</t>
+  </si>
+  <si>
+    <t>MaxSal_Assistant Director_FT</t>
+  </si>
+  <si>
+    <t>MinSal_Library Director_FT</t>
+  </si>
+  <si>
+    <t>MaxSal_Library Director_FT</t>
+  </si>
+  <si>
+    <t>MinSal_Page_PT</t>
+  </si>
+  <si>
+    <t>MaxSal_Page_PT</t>
   </si>
 </sst>
 </file>
@@ -6490,6 +6571,39 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -6498,9 +6612,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -6514,37 +6625,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -6916,8 +6997,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:GL82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="EJ1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="EP3" sqref="EP3"/>
+    <sheetView tabSelected="1" topLeftCell="FR1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="FW3" sqref="FW3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6973,277 +7054,277 @@
         <v>1879</v>
       </c>
       <c r="C2" t="s">
+        <v>1923</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1924</v>
+      </c>
+      <c r="E2" t="s">
+        <v>1925</v>
+      </c>
+      <c r="F2" t="s">
+        <v>1926</v>
+      </c>
+      <c r="G2" t="s">
+        <v>1927</v>
+      </c>
+      <c r="H2" t="s">
         <v>1928</v>
       </c>
-      <c r="D2" t="s">
+      <c r="I2" t="s">
+        <v>2006</v>
+      </c>
+      <c r="J2" t="s">
+        <v>1989</v>
+      </c>
+      <c r="K2" t="s">
+        <v>1990</v>
+      </c>
+      <c r="L2" t="s">
+        <v>1991</v>
+      </c>
+      <c r="M2" t="s">
+        <v>1992</v>
+      </c>
+      <c r="N2" t="s">
         <v>1929</v>
       </c>
-      <c r="E2" t="s">
+      <c r="O2" t="s">
         <v>1930</v>
       </c>
-      <c r="F2" t="s">
+      <c r="P2" t="s">
         <v>1931</v>
       </c>
-      <c r="G2" t="s">
+      <c r="Q2" t="s">
         <v>1932</v>
       </c>
-      <c r="H2" t="s">
+      <c r="R2" t="s">
+        <v>1993</v>
+      </c>
+      <c r="S2" t="s">
+        <v>1994</v>
+      </c>
+      <c r="T2" t="s">
+        <v>1995</v>
+      </c>
+      <c r="U2" t="s">
+        <v>1996</v>
+      </c>
+      <c r="V2" t="s">
         <v>1933</v>
       </c>
-      <c r="I2" t="s">
+      <c r="W2" t="s">
+        <v>1934</v>
+      </c>
+      <c r="X2" t="s">
+        <v>1935</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>1936</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>1937</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>1938</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>1939</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>1940</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>1941</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>1942</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>1997</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>2007</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>1943</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>1944</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>2008</v>
+      </c>
+      <c r="AK2" t="s">
+        <v>1945</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>1946</v>
+      </c>
+      <c r="AM2" t="s">
+        <v>1947</v>
+      </c>
+      <c r="AN2" t="s">
+        <v>1948</v>
+      </c>
+      <c r="AO2" t="s">
+        <v>1949</v>
+      </c>
+      <c r="AP2" t="s">
+        <v>1950</v>
+      </c>
+      <c r="AQ2" t="s">
+        <v>1951</v>
+      </c>
+      <c r="AR2" t="s">
+        <v>1952</v>
+      </c>
+      <c r="AS2" t="s">
+        <v>1953</v>
+      </c>
+      <c r="AT2" t="s">
+        <v>2001</v>
+      </c>
+      <c r="AU2" t="s">
+        <v>2000</v>
+      </c>
+      <c r="AV2" t="s">
+        <v>2002</v>
+      </c>
+      <c r="AW2" t="s">
+        <v>2003</v>
+      </c>
+      <c r="AX2" t="s">
+        <v>2004</v>
+      </c>
+      <c r="AY2" t="s">
+        <v>2005</v>
+      </c>
+      <c r="AZ2" t="s">
+        <v>1998</v>
+      </c>
+      <c r="BA2" t="s">
+        <v>1999</v>
+      </c>
+      <c r="BB2" t="s">
+        <v>1954</v>
+      </c>
+      <c r="BC2" t="s">
+        <v>1955</v>
+      </c>
+      <c r="BD2" t="s">
+        <v>1956</v>
+      </c>
+      <c r="BE2" t="s">
+        <v>1957</v>
+      </c>
+      <c r="BF2" t="s">
+        <v>2010</v>
+      </c>
+      <c r="BG2" t="s">
         <v>2011</v>
       </c>
-      <c r="J2" t="s">
-        <v>1994</v>
-      </c>
-      <c r="K2" t="s">
-        <v>1995</v>
-      </c>
-      <c r="L2" t="s">
-        <v>1996</v>
-      </c>
-      <c r="M2" t="s">
-        <v>1997</v>
-      </c>
-      <c r="N2" t="s">
-        <v>1934</v>
-      </c>
-      <c r="O2" t="s">
-        <v>1935</v>
-      </c>
-      <c r="P2" t="s">
-        <v>1936</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>1937</v>
-      </c>
-      <c r="R2" t="s">
-        <v>1998</v>
-      </c>
-      <c r="S2" t="s">
-        <v>1999</v>
-      </c>
-      <c r="T2" t="s">
-        <v>2000</v>
-      </c>
-      <c r="U2" t="s">
-        <v>2001</v>
-      </c>
-      <c r="V2" t="s">
-        <v>1938</v>
-      </c>
-      <c r="W2" t="s">
-        <v>1939</v>
-      </c>
-      <c r="X2" t="s">
-        <v>1940</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>1941</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>1942</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>1943</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>1944</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>1945</v>
-      </c>
-      <c r="AD2" t="s">
-        <v>1946</v>
-      </c>
-      <c r="AE2" t="s">
-        <v>1947</v>
-      </c>
-      <c r="AF2" t="s">
-        <v>2002</v>
-      </c>
-      <c r="AG2" t="s">
+      <c r="BH2" t="s">
         <v>2012</v>
       </c>
-      <c r="AH2" t="s">
-        <v>1948</v>
-      </c>
-      <c r="AI2" t="s">
-        <v>1949</v>
-      </c>
-      <c r="AJ2" t="s">
+      <c r="BI2" t="s">
         <v>2013</v>
       </c>
-      <c r="AK2" t="s">
-        <v>1950</v>
-      </c>
-      <c r="AL2" t="s">
-        <v>1951</v>
-      </c>
-      <c r="AM2" t="s">
-        <v>1952</v>
-      </c>
-      <c r="AN2" t="s">
-        <v>1953</v>
-      </c>
-      <c r="AO2" t="s">
-        <v>1954</v>
-      </c>
-      <c r="AP2" t="s">
-        <v>1955</v>
-      </c>
-      <c r="AQ2" t="s">
-        <v>1956</v>
-      </c>
-      <c r="AR2" t="s">
-        <v>1957</v>
-      </c>
-      <c r="AS2" t="s">
+      <c r="BJ2" t="s">
         <v>1958</v>
       </c>
-      <c r="AT2" t="s">
-        <v>2006</v>
-      </c>
-      <c r="AU2" t="s">
-        <v>2005</v>
-      </c>
-      <c r="AV2" t="s">
-        <v>2007</v>
-      </c>
-      <c r="AW2" t="s">
-        <v>2008</v>
-      </c>
-      <c r="AX2" t="s">
+      <c r="BK2" t="s">
+        <v>1959</v>
+      </c>
+      <c r="BL2" t="s">
+        <v>1960</v>
+      </c>
+      <c r="BM2" t="s">
+        <v>1961</v>
+      </c>
+      <c r="BN2" t="s">
+        <v>1962</v>
+      </c>
+      <c r="BO2" t="s">
+        <v>1963</v>
+      </c>
+      <c r="BP2" t="s">
+        <v>1964</v>
+      </c>
+      <c r="BQ2" t="s">
+        <v>1965</v>
+      </c>
+      <c r="BR2" t="s">
+        <v>1966</v>
+      </c>
+      <c r="BS2" t="s">
+        <v>1967</v>
+      </c>
+      <c r="BT2" t="s">
+        <v>1968</v>
+      </c>
+      <c r="BU2" t="s">
+        <v>1969</v>
+      </c>
+      <c r="BV2" t="s">
+        <v>1970</v>
+      </c>
+      <c r="BW2" t="s">
+        <v>1971</v>
+      </c>
+      <c r="BX2" t="s">
+        <v>1972</v>
+      </c>
+      <c r="BY2" t="s">
+        <v>1973</v>
+      </c>
+      <c r="BZ2" t="s">
+        <v>1974</v>
+      </c>
+      <c r="CA2" t="s">
+        <v>1975</v>
+      </c>
+      <c r="CB2" t="s">
+        <v>1976</v>
+      </c>
+      <c r="CC2" t="s">
+        <v>1977</v>
+      </c>
+      <c r="CD2" t="s">
         <v>2009</v>
       </c>
-      <c r="AY2" t="s">
-        <v>2010</v>
-      </c>
-      <c r="AZ2" t="s">
-        <v>2003</v>
-      </c>
-      <c r="BA2" t="s">
-        <v>2004</v>
-      </c>
-      <c r="BB2" t="s">
-        <v>1959</v>
-      </c>
-      <c r="BC2" t="s">
-        <v>1960</v>
-      </c>
-      <c r="BD2" t="s">
-        <v>1961</v>
-      </c>
-      <c r="BE2" t="s">
-        <v>1962</v>
-      </c>
-      <c r="BF2" t="s">
-        <v>2015</v>
-      </c>
-      <c r="BG2" t="s">
-        <v>2016</v>
-      </c>
-      <c r="BH2" t="s">
-        <v>2017</v>
-      </c>
-      <c r="BI2" t="s">
-        <v>2018</v>
-      </c>
-      <c r="BJ2" t="s">
-        <v>1963</v>
-      </c>
-      <c r="BK2" t="s">
-        <v>1964</v>
-      </c>
-      <c r="BL2" t="s">
-        <v>1965</v>
-      </c>
-      <c r="BM2" t="s">
-        <v>1966</v>
-      </c>
-      <c r="BN2" t="s">
-        <v>1967</v>
-      </c>
-      <c r="BO2" t="s">
-        <v>1968</v>
-      </c>
-      <c r="BP2" t="s">
-        <v>1969</v>
-      </c>
-      <c r="BQ2" t="s">
-        <v>1970</v>
-      </c>
-      <c r="BR2" t="s">
-        <v>1971</v>
-      </c>
-      <c r="BS2" t="s">
-        <v>1972</v>
-      </c>
-      <c r="BT2" t="s">
-        <v>1973</v>
-      </c>
-      <c r="BU2" t="s">
-        <v>1974</v>
-      </c>
-      <c r="BV2" t="s">
-        <v>1975</v>
-      </c>
-      <c r="BW2" t="s">
-        <v>1976</v>
-      </c>
-      <c r="BX2" t="s">
-        <v>1977</v>
-      </c>
-      <c r="BY2" t="s">
+      <c r="CE2" t="s">
         <v>1978</v>
       </c>
-      <c r="BZ2" t="s">
+      <c r="CF2" t="s">
         <v>1979</v>
       </c>
-      <c r="CA2" t="s">
+      <c r="CG2" t="s">
         <v>1980</v>
       </c>
-      <c r="CB2" t="s">
+      <c r="CH2" t="s">
         <v>1981</v>
       </c>
-      <c r="CC2" t="s">
+      <c r="CI2" t="s">
         <v>1982</v>
       </c>
-      <c r="CD2" t="s">
-        <v>2014</v>
-      </c>
-      <c r="CE2" t="s">
+      <c r="CJ2" t="s">
         <v>1983</v>
       </c>
-      <c r="CF2" t="s">
+      <c r="CK2" t="s">
         <v>1984</v>
       </c>
-      <c r="CG2" t="s">
+      <c r="CL2" t="s">
         <v>1985</v>
       </c>
-      <c r="CH2" t="s">
+      <c r="CM2" t="s">
         <v>1986</v>
       </c>
-      <c r="CI2" t="s">
+      <c r="CN2" t="s">
         <v>1987</v>
       </c>
-      <c r="CJ2" t="s">
+      <c r="CO2" t="s">
         <v>1988</v>
-      </c>
-      <c r="CK2" t="s">
-        <v>1989</v>
-      </c>
-      <c r="CL2" t="s">
-        <v>1990</v>
-      </c>
-      <c r="CM2" t="s">
-        <v>1991</v>
-      </c>
-      <c r="CN2" t="s">
-        <v>1992</v>
-      </c>
-      <c r="CO2" t="s">
-        <v>1993</v>
       </c>
       <c r="CP2" t="s">
         <v>23</v>
@@ -7348,160 +7429,160 @@
         <v>557</v>
       </c>
       <c r="DX2" t="s">
+        <v>2017</v>
+      </c>
+      <c r="DY2" t="s">
+        <v>2016</v>
+      </c>
+      <c r="DZ2" t="s">
+        <v>2014</v>
+      </c>
+      <c r="EA2" t="s">
+        <v>2015</v>
+      </c>
+      <c r="EB2" t="s">
+        <v>2018</v>
+      </c>
+      <c r="EC2" t="s">
+        <v>2019</v>
+      </c>
+      <c r="ED2" t="s">
+        <v>2020</v>
+      </c>
+      <c r="EE2" t="s">
+        <v>2021</v>
+      </c>
+      <c r="EF2" t="s">
         <v>2022</v>
       </c>
-      <c r="DY2" t="s">
-        <v>2021</v>
-      </c>
-      <c r="DZ2" t="s">
-        <v>2019</v>
-      </c>
-      <c r="EA2" t="s">
-        <v>2020</v>
-      </c>
-      <c r="EB2" t="s">
+      <c r="EG2" t="s">
         <v>2023</v>
       </c>
-      <c r="EC2" t="s">
+      <c r="EH2" t="s">
         <v>2024</v>
       </c>
-      <c r="ED2" t="s">
+      <c r="EI2" t="s">
         <v>2025</v>
       </c>
-      <c r="EE2" t="s">
+      <c r="EJ2" t="s">
         <v>2026</v>
       </c>
-      <c r="EF2" t="s">
+      <c r="EK2" t="s">
         <v>2027</v>
       </c>
-      <c r="EG2" t="s">
+      <c r="EL2" t="s">
         <v>2028</v>
       </c>
-      <c r="EH2" t="s">
+      <c r="EM2" t="s">
         <v>2029</v>
       </c>
-      <c r="EI2" t="s">
+      <c r="EN2" t="s">
         <v>2030</v>
       </c>
-      <c r="EJ2" t="s">
+      <c r="EO2" t="s">
         <v>2031</v>
       </c>
-      <c r="EK2" t="s">
+      <c r="EP2" t="s">
         <v>2032</v>
       </c>
-      <c r="EL2" t="s">
+      <c r="EQ2" t="s">
         <v>2033</v>
       </c>
-      <c r="EM2" t="s">
+      <c r="ER2" t="s">
         <v>2034</v>
       </c>
-      <c r="EN2" t="s">
+      <c r="ES2" t="s">
         <v>2035</v>
       </c>
-      <c r="EO2" t="s">
+      <c r="ET2" t="s">
         <v>2036</v>
       </c>
-      <c r="EP2" t="s">
+      <c r="EU2" t="s">
         <v>2037</v>
       </c>
-      <c r="EQ2" t="s">
+      <c r="EV2" t="s">
         <v>2038</v>
       </c>
-      <c r="ER2" t="s">
-        <v>659</v>
-      </c>
-      <c r="ES2" t="s">
-        <v>660</v>
-      </c>
-      <c r="ET2" t="s">
-        <v>560</v>
-      </c>
-      <c r="EU2" t="s">
-        <v>1885</v>
-      </c>
-      <c r="EV2" t="s">
-        <v>662</v>
-      </c>
       <c r="EW2" t="s">
-        <v>663</v>
+        <v>2039</v>
       </c>
       <c r="EX2" t="s">
-        <v>665</v>
+        <v>2040</v>
       </c>
       <c r="EY2" t="s">
-        <v>1886</v>
+        <v>2041</v>
       </c>
       <c r="EZ2" t="s">
-        <v>668</v>
+        <v>2042</v>
       </c>
       <c r="FA2" t="s">
-        <v>669</v>
+        <v>2043</v>
       </c>
       <c r="FB2" t="s">
-        <v>729</v>
+        <v>2044</v>
       </c>
       <c r="FC2" t="s">
-        <v>730</v>
+        <v>2045</v>
       </c>
       <c r="FD2" t="s">
-        <v>872</v>
+        <v>2046</v>
       </c>
       <c r="FE2" t="s">
-        <v>1887</v>
+        <v>2047</v>
       </c>
       <c r="FF2" t="s">
-        <v>887</v>
+        <v>2048</v>
       </c>
       <c r="FG2" t="s">
-        <v>888</v>
+        <v>2049</v>
       </c>
       <c r="FH2" t="s">
-        <v>597</v>
+        <v>2050</v>
       </c>
       <c r="FI2" t="s">
-        <v>1888</v>
+        <v>2051</v>
       </c>
       <c r="FJ2" t="s">
-        <v>598</v>
+        <v>2052</v>
       </c>
       <c r="FK2" t="s">
-        <v>890</v>
+        <v>2053</v>
       </c>
       <c r="FL2" t="s">
-        <v>894</v>
+        <v>2054</v>
       </c>
       <c r="FM2" t="s">
-        <v>895</v>
+        <v>2055</v>
       </c>
       <c r="FN2" t="s">
-        <v>601</v>
+        <v>2056</v>
       </c>
       <c r="FO2" t="s">
-        <v>602</v>
+        <v>2057</v>
       </c>
       <c r="FP2" t="s">
-        <v>943</v>
+        <v>2058</v>
       </c>
       <c r="FQ2" t="s">
-        <v>944</v>
+        <v>2059</v>
       </c>
       <c r="FR2" t="s">
-        <v>609</v>
+        <v>2060</v>
       </c>
       <c r="FS2" t="s">
-        <v>976</v>
+        <v>2061</v>
       </c>
       <c r="FT2" t="s">
-        <v>981</v>
+        <v>2062</v>
       </c>
       <c r="FU2" t="s">
-        <v>982</v>
+        <v>2063</v>
       </c>
       <c r="FV2" t="s">
-        <v>610</v>
+        <v>2064</v>
       </c>
       <c r="FW2" t="s">
-        <v>1889</v>
+        <v>2065</v>
       </c>
     </row>
     <row r="3" spans="1:194" x14ac:dyDescent="0.35">
@@ -18152,753 +18233,753 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:785 16376:16376" s="25" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="51" t="s">
+      <c r="A2" s="62" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="57" t="s">
+      <c r="B2" s="67" t="s">
         <v>448</v>
       </c>
-      <c r="C2" s="57"/>
-      <c r="D2" s="54" t="s">
+      <c r="C2" s="67"/>
+      <c r="D2" s="64" t="s">
         <v>449</v>
       </c>
-      <c r="E2" s="54"/>
-      <c r="F2" s="54"/>
-      <c r="G2" s="54"/>
-      <c r="H2" s="54"/>
-      <c r="I2" s="54"/>
-      <c r="J2" s="54"/>
-      <c r="K2" s="54"/>
-      <c r="L2" s="54"/>
-      <c r="M2" s="54"/>
-      <c r="N2" s="54"/>
-      <c r="O2" s="54"/>
-      <c r="P2" s="54"/>
-      <c r="Q2" s="55" t="s">
+      <c r="E2" s="64"/>
+      <c r="F2" s="64"/>
+      <c r="G2" s="64"/>
+      <c r="H2" s="64"/>
+      <c r="I2" s="64"/>
+      <c r="J2" s="64"/>
+      <c r="K2" s="64"/>
+      <c r="L2" s="64"/>
+      <c r="M2" s="64"/>
+      <c r="N2" s="64"/>
+      <c r="O2" s="64"/>
+      <c r="P2" s="64"/>
+      <c r="Q2" s="65" t="s">
         <v>450</v>
       </c>
-      <c r="R2" s="55"/>
-      <c r="S2" s="55"/>
-      <c r="T2" s="55"/>
-      <c r="U2" s="55"/>
-      <c r="V2" s="55"/>
-      <c r="W2" s="55"/>
-      <c r="X2" s="55"/>
-      <c r="Y2" s="55"/>
-      <c r="Z2" s="55"/>
-      <c r="AA2" s="55"/>
-      <c r="AB2" s="55"/>
-      <c r="AC2" s="55"/>
-      <c r="AD2" s="55"/>
-      <c r="AE2" s="55"/>
-      <c r="AF2" s="55"/>
-      <c r="AG2" s="56" t="s">
+      <c r="R2" s="65"/>
+      <c r="S2" s="65"/>
+      <c r="T2" s="65"/>
+      <c r="U2" s="65"/>
+      <c r="V2" s="65"/>
+      <c r="W2" s="65"/>
+      <c r="X2" s="65"/>
+      <c r="Y2" s="65"/>
+      <c r="Z2" s="65"/>
+      <c r="AA2" s="65"/>
+      <c r="AB2" s="65"/>
+      <c r="AC2" s="65"/>
+      <c r="AD2" s="65"/>
+      <c r="AE2" s="65"/>
+      <c r="AF2" s="65"/>
+      <c r="AG2" s="66" t="s">
         <v>451</v>
       </c>
-      <c r="AH2" s="56"/>
-      <c r="AI2" s="56"/>
-      <c r="AJ2" s="56"/>
-      <c r="AK2" s="56"/>
-      <c r="AL2" s="56"/>
-      <c r="AM2" s="56"/>
-      <c r="AN2" s="56"/>
-      <c r="AO2" s="56"/>
-      <c r="AP2" s="56"/>
-      <c r="AQ2" s="56"/>
-      <c r="AR2" s="56"/>
-      <c r="AS2" s="56"/>
-      <c r="AT2" s="56"/>
-      <c r="AU2" s="56"/>
-      <c r="AV2" s="56"/>
-      <c r="AW2" s="56"/>
-      <c r="AX2" s="56"/>
-      <c r="AY2" s="56"/>
-      <c r="AZ2" s="56"/>
-      <c r="BA2" s="53" t="s">
+      <c r="AH2" s="66"/>
+      <c r="AI2" s="66"/>
+      <c r="AJ2" s="66"/>
+      <c r="AK2" s="66"/>
+      <c r="AL2" s="66"/>
+      <c r="AM2" s="66"/>
+      <c r="AN2" s="66"/>
+      <c r="AO2" s="66"/>
+      <c r="AP2" s="66"/>
+      <c r="AQ2" s="66"/>
+      <c r="AR2" s="66"/>
+      <c r="AS2" s="66"/>
+      <c r="AT2" s="66"/>
+      <c r="AU2" s="66"/>
+      <c r="AV2" s="66"/>
+      <c r="AW2" s="66"/>
+      <c r="AX2" s="66"/>
+      <c r="AY2" s="66"/>
+      <c r="AZ2" s="66"/>
+      <c r="BA2" s="55" t="s">
         <v>452</v>
       </c>
-      <c r="BB2" s="53"/>
-      <c r="BC2" s="53"/>
-      <c r="BD2" s="53"/>
-      <c r="BE2" s="53"/>
-      <c r="BF2" s="53"/>
-      <c r="BG2" s="53"/>
-      <c r="BH2" s="53"/>
-      <c r="BI2" s="53"/>
-      <c r="BJ2" s="53"/>
-      <c r="BK2" s="53"/>
-      <c r="BL2" s="53"/>
-      <c r="BM2" s="53"/>
-      <c r="BN2" s="53"/>
-      <c r="BO2" s="53"/>
-      <c r="BP2" s="53"/>
-      <c r="BQ2" s="53"/>
-      <c r="BR2" s="53"/>
-      <c r="BS2" s="53"/>
-      <c r="BT2" s="53"/>
-      <c r="BU2" s="53"/>
-      <c r="BV2" s="53"/>
-      <c r="BW2" s="53"/>
-      <c r="BX2" s="53"/>
-      <c r="BY2" s="53"/>
-      <c r="BZ2" s="53"/>
-      <c r="CA2" s="53"/>
-      <c r="CB2" s="53"/>
-      <c r="CC2" s="53"/>
-      <c r="CD2" s="53"/>
-      <c r="CE2" s="53"/>
-      <c r="CF2" s="53"/>
-      <c r="CG2" s="53"/>
-      <c r="CH2" s="53"/>
-      <c r="CI2" s="53"/>
-      <c r="CJ2" s="53"/>
-      <c r="CK2" s="55" t="s">
+      <c r="BB2" s="55"/>
+      <c r="BC2" s="55"/>
+      <c r="BD2" s="55"/>
+      <c r="BE2" s="55"/>
+      <c r="BF2" s="55"/>
+      <c r="BG2" s="55"/>
+      <c r="BH2" s="55"/>
+      <c r="BI2" s="55"/>
+      <c r="BJ2" s="55"/>
+      <c r="BK2" s="55"/>
+      <c r="BL2" s="55"/>
+      <c r="BM2" s="55"/>
+      <c r="BN2" s="55"/>
+      <c r="BO2" s="55"/>
+      <c r="BP2" s="55"/>
+      <c r="BQ2" s="55"/>
+      <c r="BR2" s="55"/>
+      <c r="BS2" s="55"/>
+      <c r="BT2" s="55"/>
+      <c r="BU2" s="55"/>
+      <c r="BV2" s="55"/>
+      <c r="BW2" s="55"/>
+      <c r="BX2" s="55"/>
+      <c r="BY2" s="55"/>
+      <c r="BZ2" s="55"/>
+      <c r="CA2" s="55"/>
+      <c r="CB2" s="55"/>
+      <c r="CC2" s="55"/>
+      <c r="CD2" s="55"/>
+      <c r="CE2" s="55"/>
+      <c r="CF2" s="55"/>
+      <c r="CG2" s="55"/>
+      <c r="CH2" s="55"/>
+      <c r="CI2" s="55"/>
+      <c r="CJ2" s="55"/>
+      <c r="CK2" s="65" t="s">
         <v>453</v>
       </c>
-      <c r="CL2" s="55"/>
-      <c r="CM2" s="55"/>
-      <c r="CN2" s="55"/>
-      <c r="CO2" s="55"/>
-      <c r="CP2" s="55"/>
-      <c r="CQ2" s="55"/>
-      <c r="CR2" s="55"/>
-      <c r="CS2" s="55"/>
-      <c r="CT2" s="55"/>
-      <c r="CU2" s="55"/>
-      <c r="CV2" s="55"/>
-      <c r="CW2" s="55"/>
-      <c r="CX2" s="55"/>
-      <c r="CY2" s="55"/>
-      <c r="CZ2" s="55"/>
-      <c r="DA2" s="55"/>
-      <c r="DB2" s="55"/>
-      <c r="DC2" s="55"/>
-      <c r="DD2" s="55"/>
-      <c r="DE2" s="55"/>
-      <c r="DF2" s="55"/>
-      <c r="DG2" s="55"/>
-      <c r="DH2" s="55"/>
-      <c r="DI2" s="55"/>
-      <c r="DJ2" s="55"/>
-      <c r="DK2" s="55"/>
-      <c r="DL2" s="55"/>
-      <c r="DM2" s="55"/>
-      <c r="DN2" s="55"/>
-      <c r="DO2" s="55"/>
-      <c r="DP2" s="55"/>
-      <c r="DQ2" s="55"/>
-      <c r="DR2" s="55"/>
-      <c r="DS2" s="55"/>
-      <c r="DT2" s="55"/>
-      <c r="DU2" s="55"/>
-      <c r="DV2" s="55"/>
-      <c r="DW2" s="55"/>
-      <c r="DX2" s="55"/>
-      <c r="DY2" s="61" t="s">
+      <c r="CL2" s="65"/>
+      <c r="CM2" s="65"/>
+      <c r="CN2" s="65"/>
+      <c r="CO2" s="65"/>
+      <c r="CP2" s="65"/>
+      <c r="CQ2" s="65"/>
+      <c r="CR2" s="65"/>
+      <c r="CS2" s="65"/>
+      <c r="CT2" s="65"/>
+      <c r="CU2" s="65"/>
+      <c r="CV2" s="65"/>
+      <c r="CW2" s="65"/>
+      <c r="CX2" s="65"/>
+      <c r="CY2" s="65"/>
+      <c r="CZ2" s="65"/>
+      <c r="DA2" s="65"/>
+      <c r="DB2" s="65"/>
+      <c r="DC2" s="65"/>
+      <c r="DD2" s="65"/>
+      <c r="DE2" s="65"/>
+      <c r="DF2" s="65"/>
+      <c r="DG2" s="65"/>
+      <c r="DH2" s="65"/>
+      <c r="DI2" s="65"/>
+      <c r="DJ2" s="65"/>
+      <c r="DK2" s="65"/>
+      <c r="DL2" s="65"/>
+      <c r="DM2" s="65"/>
+      <c r="DN2" s="65"/>
+      <c r="DO2" s="65"/>
+      <c r="DP2" s="65"/>
+      <c r="DQ2" s="65"/>
+      <c r="DR2" s="65"/>
+      <c r="DS2" s="65"/>
+      <c r="DT2" s="65"/>
+      <c r="DU2" s="65"/>
+      <c r="DV2" s="65"/>
+      <c r="DW2" s="65"/>
+      <c r="DX2" s="65"/>
+      <c r="DY2" s="57" t="s">
         <v>454</v>
       </c>
-      <c r="DZ2" s="61"/>
-      <c r="EA2" s="61"/>
-      <c r="EB2" s="61"/>
-      <c r="EC2" s="61"/>
-      <c r="ED2" s="61"/>
-      <c r="EE2" s="61"/>
-      <c r="EF2" s="61"/>
-      <c r="EG2" s="61"/>
-      <c r="EH2" s="61"/>
-      <c r="EI2" s="61"/>
-      <c r="EJ2" s="61"/>
-      <c r="EK2" s="61"/>
-      <c r="EL2" s="61"/>
-      <c r="EM2" s="61"/>
-      <c r="EN2" s="61"/>
-      <c r="EO2" s="61"/>
-      <c r="EP2" s="61"/>
-      <c r="EQ2" s="61"/>
-      <c r="ER2" s="61"/>
-      <c r="ES2" s="61"/>
-      <c r="ET2" s="61"/>
-      <c r="EU2" s="61"/>
-      <c r="EV2" s="61"/>
-      <c r="EW2" s="61"/>
-      <c r="EX2" s="61"/>
-      <c r="EY2" s="61"/>
-      <c r="EZ2" s="61"/>
-      <c r="FA2" s="61"/>
-      <c r="FB2" s="62" t="s">
+      <c r="DZ2" s="57"/>
+      <c r="EA2" s="57"/>
+      <c r="EB2" s="57"/>
+      <c r="EC2" s="57"/>
+      <c r="ED2" s="57"/>
+      <c r="EE2" s="57"/>
+      <c r="EF2" s="57"/>
+      <c r="EG2" s="57"/>
+      <c r="EH2" s="57"/>
+      <c r="EI2" s="57"/>
+      <c r="EJ2" s="57"/>
+      <c r="EK2" s="57"/>
+      <c r="EL2" s="57"/>
+      <c r="EM2" s="57"/>
+      <c r="EN2" s="57"/>
+      <c r="EO2" s="57"/>
+      <c r="EP2" s="57"/>
+      <c r="EQ2" s="57"/>
+      <c r="ER2" s="57"/>
+      <c r="ES2" s="57"/>
+      <c r="ET2" s="57"/>
+      <c r="EU2" s="57"/>
+      <c r="EV2" s="57"/>
+      <c r="EW2" s="57"/>
+      <c r="EX2" s="57"/>
+      <c r="EY2" s="57"/>
+      <c r="EZ2" s="57"/>
+      <c r="FA2" s="57"/>
+      <c r="FB2" s="54" t="s">
         <v>487</v>
       </c>
-      <c r="FC2" s="62"/>
-      <c r="FD2" s="62"/>
-      <c r="FE2" s="62"/>
-      <c r="FF2" s="63" t="s">
+      <c r="FC2" s="54"/>
+      <c r="FD2" s="54"/>
+      <c r="FE2" s="54"/>
+      <c r="FF2" s="58" t="s">
         <v>488</v>
       </c>
-      <c r="FG2" s="63"/>
-      <c r="FH2" s="63"/>
-      <c r="FI2" s="63"/>
-      <c r="FJ2" s="63"/>
-      <c r="FK2" s="63"/>
-      <c r="FL2" s="63"/>
-      <c r="FM2" s="63"/>
-      <c r="FN2" s="63"/>
-      <c r="FO2" s="63"/>
-      <c r="FP2" s="63"/>
-      <c r="FQ2" s="63"/>
-      <c r="FR2" s="63"/>
-      <c r="FS2" s="63"/>
-      <c r="FT2" s="63"/>
-      <c r="FU2" s="63"/>
-      <c r="FV2" s="63"/>
-      <c r="FW2" s="63"/>
-      <c r="FX2" s="63"/>
-      <c r="FY2" s="63"/>
-      <c r="FZ2" s="63"/>
-      <c r="GA2" s="63"/>
-      <c r="GB2" s="64" t="s">
+      <c r="FG2" s="58"/>
+      <c r="FH2" s="58"/>
+      <c r="FI2" s="58"/>
+      <c r="FJ2" s="58"/>
+      <c r="FK2" s="58"/>
+      <c r="FL2" s="58"/>
+      <c r="FM2" s="58"/>
+      <c r="FN2" s="58"/>
+      <c r="FO2" s="58"/>
+      <c r="FP2" s="58"/>
+      <c r="FQ2" s="58"/>
+      <c r="FR2" s="58"/>
+      <c r="FS2" s="58"/>
+      <c r="FT2" s="58"/>
+      <c r="FU2" s="58"/>
+      <c r="FV2" s="58"/>
+      <c r="FW2" s="58"/>
+      <c r="FX2" s="58"/>
+      <c r="FY2" s="58"/>
+      <c r="FZ2" s="58"/>
+      <c r="GA2" s="58"/>
+      <c r="GB2" s="59" t="s">
         <v>489</v>
       </c>
-      <c r="GC2" s="64"/>
-      <c r="GD2" s="64"/>
-      <c r="GE2" s="64"/>
-      <c r="GF2" s="64"/>
-      <c r="GG2" s="64"/>
-      <c r="GH2" s="64"/>
-      <c r="GI2" s="64"/>
-      <c r="GJ2" s="64"/>
-      <c r="GK2" s="64"/>
-      <c r="GL2" s="64"/>
-      <c r="GM2" s="65" t="s">
+      <c r="GC2" s="59"/>
+      <c r="GD2" s="59"/>
+      <c r="GE2" s="59"/>
+      <c r="GF2" s="59"/>
+      <c r="GG2" s="59"/>
+      <c r="GH2" s="59"/>
+      <c r="GI2" s="59"/>
+      <c r="GJ2" s="59"/>
+      <c r="GK2" s="59"/>
+      <c r="GL2" s="59"/>
+      <c r="GM2" s="60" t="s">
         <v>490</v>
       </c>
-      <c r="GN2" s="65"/>
-      <c r="GO2" s="65"/>
-      <c r="GP2" s="65"/>
-      <c r="GQ2" s="65"/>
-      <c r="GR2" s="65"/>
-      <c r="GS2" s="65"/>
-      <c r="GT2" s="65"/>
-      <c r="GU2" s="65"/>
-      <c r="GV2" s="65"/>
-      <c r="GW2" s="65"/>
-      <c r="GX2" s="65"/>
-      <c r="GY2" s="65"/>
-      <c r="GZ2" s="65"/>
-      <c r="HA2" s="65"/>
-      <c r="HB2" s="65"/>
-      <c r="HC2" s="65"/>
-      <c r="HD2" s="65"/>
-      <c r="HE2" s="65"/>
-      <c r="HF2" s="65"/>
-      <c r="HG2" s="65"/>
-      <c r="HH2" s="65"/>
-      <c r="HI2" s="65"/>
-      <c r="HJ2" s="65"/>
-      <c r="HK2" s="65"/>
-      <c r="HL2" s="65"/>
-      <c r="HM2" s="65"/>
-      <c r="HN2" s="65"/>
-      <c r="HO2" s="65"/>
-      <c r="HP2" s="58" t="s">
+      <c r="GN2" s="60"/>
+      <c r="GO2" s="60"/>
+      <c r="GP2" s="60"/>
+      <c r="GQ2" s="60"/>
+      <c r="GR2" s="60"/>
+      <c r="GS2" s="60"/>
+      <c r="GT2" s="60"/>
+      <c r="GU2" s="60"/>
+      <c r="GV2" s="60"/>
+      <c r="GW2" s="60"/>
+      <c r="GX2" s="60"/>
+      <c r="GY2" s="60"/>
+      <c r="GZ2" s="60"/>
+      <c r="HA2" s="60"/>
+      <c r="HB2" s="60"/>
+      <c r="HC2" s="60"/>
+      <c r="HD2" s="60"/>
+      <c r="HE2" s="60"/>
+      <c r="HF2" s="60"/>
+      <c r="HG2" s="60"/>
+      <c r="HH2" s="60"/>
+      <c r="HI2" s="60"/>
+      <c r="HJ2" s="60"/>
+      <c r="HK2" s="60"/>
+      <c r="HL2" s="60"/>
+      <c r="HM2" s="60"/>
+      <c r="HN2" s="60"/>
+      <c r="HO2" s="60"/>
+      <c r="HP2" s="53" t="s">
         <v>492</v>
       </c>
-      <c r="HQ2" s="58"/>
-      <c r="HR2" s="58"/>
-      <c r="HS2" s="58"/>
-      <c r="HT2" s="58"/>
-      <c r="HU2" s="58"/>
-      <c r="HV2" s="58"/>
-      <c r="HW2" s="58"/>
-      <c r="HX2" s="58"/>
-      <c r="HY2" s="58"/>
-      <c r="HZ2" s="58"/>
-      <c r="IA2" s="58"/>
-      <c r="IB2" s="58"/>
-      <c r="IC2" s="58"/>
-      <c r="ID2" s="59" t="s">
+      <c r="HQ2" s="53"/>
+      <c r="HR2" s="53"/>
+      <c r="HS2" s="53"/>
+      <c r="HT2" s="53"/>
+      <c r="HU2" s="53"/>
+      <c r="HV2" s="53"/>
+      <c r="HW2" s="53"/>
+      <c r="HX2" s="53"/>
+      <c r="HY2" s="53"/>
+      <c r="HZ2" s="53"/>
+      <c r="IA2" s="53"/>
+      <c r="IB2" s="53"/>
+      <c r="IC2" s="53"/>
+      <c r="ID2" s="68" t="s">
         <v>493</v>
       </c>
-      <c r="IE2" s="59"/>
-      <c r="IF2" s="59"/>
-      <c r="IG2" s="59"/>
-      <c r="IH2" s="59"/>
-      <c r="II2" s="59"/>
-      <c r="IJ2" s="59"/>
-      <c r="IK2" s="59"/>
-      <c r="IL2" s="59"/>
-      <c r="IM2" s="59"/>
-      <c r="IN2" s="59"/>
-      <c r="IO2" s="59"/>
-      <c r="IP2" s="60" t="s">
+      <c r="IE2" s="68"/>
+      <c r="IF2" s="68"/>
+      <c r="IG2" s="68"/>
+      <c r="IH2" s="68"/>
+      <c r="II2" s="68"/>
+      <c r="IJ2" s="68"/>
+      <c r="IK2" s="68"/>
+      <c r="IL2" s="68"/>
+      <c r="IM2" s="68"/>
+      <c r="IN2" s="68"/>
+      <c r="IO2" s="68"/>
+      <c r="IP2" s="52" t="s">
         <v>569</v>
       </c>
-      <c r="IQ2" s="60"/>
-      <c r="IR2" s="60"/>
-      <c r="IS2" s="60"/>
-      <c r="IT2" s="60"/>
-      <c r="IU2" s="60"/>
-      <c r="IV2" s="60"/>
-      <c r="IW2" s="60"/>
-      <c r="IX2" s="60"/>
-      <c r="IY2" s="60"/>
-      <c r="IZ2" s="60"/>
-      <c r="JA2" s="60"/>
-      <c r="JB2" s="60"/>
-      <c r="JC2" s="60"/>
-      <c r="JD2" s="60"/>
-      <c r="JE2" s="60"/>
-      <c r="JF2" s="60"/>
-      <c r="JG2" s="60"/>
-      <c r="JH2" s="60"/>
-      <c r="JI2" s="60"/>
-      <c r="JJ2" s="60"/>
-      <c r="JK2" s="60"/>
-      <c r="JL2" s="60"/>
-      <c r="JM2" s="60"/>
-      <c r="JN2" s="60"/>
-      <c r="JO2" s="60"/>
-      <c r="JP2" s="60"/>
-      <c r="JQ2" s="60"/>
-      <c r="JR2" s="60"/>
-      <c r="JS2" s="60"/>
-      <c r="JT2" s="66" t="s">
+      <c r="IQ2" s="52"/>
+      <c r="IR2" s="52"/>
+      <c r="IS2" s="52"/>
+      <c r="IT2" s="52"/>
+      <c r="IU2" s="52"/>
+      <c r="IV2" s="52"/>
+      <c r="IW2" s="52"/>
+      <c r="IX2" s="52"/>
+      <c r="IY2" s="52"/>
+      <c r="IZ2" s="52"/>
+      <c r="JA2" s="52"/>
+      <c r="JB2" s="52"/>
+      <c r="JC2" s="52"/>
+      <c r="JD2" s="52"/>
+      <c r="JE2" s="52"/>
+      <c r="JF2" s="52"/>
+      <c r="JG2" s="52"/>
+      <c r="JH2" s="52"/>
+      <c r="JI2" s="52"/>
+      <c r="JJ2" s="52"/>
+      <c r="JK2" s="52"/>
+      <c r="JL2" s="52"/>
+      <c r="JM2" s="52"/>
+      <c r="JN2" s="52"/>
+      <c r="JO2" s="52"/>
+      <c r="JP2" s="52"/>
+      <c r="JQ2" s="52"/>
+      <c r="JR2" s="52"/>
+      <c r="JS2" s="52"/>
+      <c r="JT2" s="50" t="s">
         <v>570</v>
       </c>
-      <c r="JU2" s="66"/>
-      <c r="JV2" s="66"/>
-      <c r="JW2" s="66"/>
-      <c r="JX2" s="66"/>
-      <c r="JY2" s="66"/>
-      <c r="JZ2" s="66"/>
-      <c r="KA2" s="66"/>
-      <c r="KB2" s="66"/>
-      <c r="KC2" s="66"/>
-      <c r="KD2" s="66"/>
-      <c r="KE2" s="66"/>
-      <c r="KF2" s="66"/>
-      <c r="KG2" s="66"/>
-      <c r="KH2" s="66"/>
-      <c r="KI2" s="66"/>
-      <c r="KJ2" s="66"/>
-      <c r="KK2" s="66"/>
-      <c r="KL2" s="66"/>
-      <c r="KM2" s="66"/>
-      <c r="KN2" s="66"/>
-      <c r="KO2" s="66"/>
-      <c r="KP2" s="66"/>
-      <c r="KQ2" s="66"/>
-      <c r="KR2" s="66"/>
-      <c r="KS2" s="66"/>
-      <c r="KT2" s="66"/>
-      <c r="KU2" s="66"/>
-      <c r="KV2" s="66"/>
-      <c r="KW2" s="66"/>
-      <c r="KX2" s="66"/>
-      <c r="KY2" s="66"/>
-      <c r="KZ2" s="66"/>
-      <c r="LA2" s="66"/>
-      <c r="LB2" s="66"/>
-      <c r="LC2" s="66"/>
-      <c r="LD2" s="66"/>
-      <c r="LE2" s="66"/>
-      <c r="LF2" s="66"/>
-      <c r="LG2" s="66"/>
-      <c r="LH2" s="66"/>
-      <c r="LI2" s="66"/>
-      <c r="LJ2" s="66"/>
-      <c r="LK2" s="66"/>
-      <c r="LL2" s="66"/>
-      <c r="LM2" s="66"/>
-      <c r="LN2" s="66"/>
-      <c r="LO2" s="66"/>
-      <c r="LP2" s="66"/>
-      <c r="LQ2" s="66"/>
-      <c r="LR2" s="66"/>
-      <c r="LS2" s="66"/>
-      <c r="LT2" s="66"/>
-      <c r="LU2" s="66"/>
-      <c r="LV2" s="66"/>
-      <c r="LW2" s="66"/>
-      <c r="LX2" s="66"/>
-      <c r="LY2" s="66"/>
-      <c r="LZ2" s="66"/>
-      <c r="MA2" s="66"/>
-      <c r="MB2" s="66"/>
-      <c r="MC2" s="66"/>
-      <c r="MD2" s="66"/>
-      <c r="ME2" s="66"/>
-      <c r="MF2" s="66"/>
-      <c r="MG2" s="66"/>
-      <c r="MH2" s="66"/>
-      <c r="MI2" s="66"/>
-      <c r="MJ2" s="66"/>
-      <c r="MK2" s="66"/>
-      <c r="ML2" s="66"/>
-      <c r="MM2" s="66"/>
-      <c r="MN2" s="66"/>
-      <c r="MO2" s="66"/>
-      <c r="MP2" s="66"/>
-      <c r="MQ2" s="66"/>
-      <c r="MR2" s="66"/>
-      <c r="MS2" s="66"/>
-      <c r="MT2" s="66"/>
-      <c r="MU2" s="66"/>
-      <c r="MV2" s="66"/>
-      <c r="MW2" s="66"/>
-      <c r="MX2" s="66"/>
-      <c r="MY2" s="66"/>
-      <c r="MZ2" s="66"/>
-      <c r="NA2" s="66"/>
-      <c r="NB2" s="66"/>
-      <c r="NC2" s="66"/>
-      <c r="ND2" s="66"/>
-      <c r="NE2" s="66"/>
-      <c r="NF2" s="67" t="s">
+      <c r="JU2" s="50"/>
+      <c r="JV2" s="50"/>
+      <c r="JW2" s="50"/>
+      <c r="JX2" s="50"/>
+      <c r="JY2" s="50"/>
+      <c r="JZ2" s="50"/>
+      <c r="KA2" s="50"/>
+      <c r="KB2" s="50"/>
+      <c r="KC2" s="50"/>
+      <c r="KD2" s="50"/>
+      <c r="KE2" s="50"/>
+      <c r="KF2" s="50"/>
+      <c r="KG2" s="50"/>
+      <c r="KH2" s="50"/>
+      <c r="KI2" s="50"/>
+      <c r="KJ2" s="50"/>
+      <c r="KK2" s="50"/>
+      <c r="KL2" s="50"/>
+      <c r="KM2" s="50"/>
+      <c r="KN2" s="50"/>
+      <c r="KO2" s="50"/>
+      <c r="KP2" s="50"/>
+      <c r="KQ2" s="50"/>
+      <c r="KR2" s="50"/>
+      <c r="KS2" s="50"/>
+      <c r="KT2" s="50"/>
+      <c r="KU2" s="50"/>
+      <c r="KV2" s="50"/>
+      <c r="KW2" s="50"/>
+      <c r="KX2" s="50"/>
+      <c r="KY2" s="50"/>
+      <c r="KZ2" s="50"/>
+      <c r="LA2" s="50"/>
+      <c r="LB2" s="50"/>
+      <c r="LC2" s="50"/>
+      <c r="LD2" s="50"/>
+      <c r="LE2" s="50"/>
+      <c r="LF2" s="50"/>
+      <c r="LG2" s="50"/>
+      <c r="LH2" s="50"/>
+      <c r="LI2" s="50"/>
+      <c r="LJ2" s="50"/>
+      <c r="LK2" s="50"/>
+      <c r="LL2" s="50"/>
+      <c r="LM2" s="50"/>
+      <c r="LN2" s="50"/>
+      <c r="LO2" s="50"/>
+      <c r="LP2" s="50"/>
+      <c r="LQ2" s="50"/>
+      <c r="LR2" s="50"/>
+      <c r="LS2" s="50"/>
+      <c r="LT2" s="50"/>
+      <c r="LU2" s="50"/>
+      <c r="LV2" s="50"/>
+      <c r="LW2" s="50"/>
+      <c r="LX2" s="50"/>
+      <c r="LY2" s="50"/>
+      <c r="LZ2" s="50"/>
+      <c r="MA2" s="50"/>
+      <c r="MB2" s="50"/>
+      <c r="MC2" s="50"/>
+      <c r="MD2" s="50"/>
+      <c r="ME2" s="50"/>
+      <c r="MF2" s="50"/>
+      <c r="MG2" s="50"/>
+      <c r="MH2" s="50"/>
+      <c r="MI2" s="50"/>
+      <c r="MJ2" s="50"/>
+      <c r="MK2" s="50"/>
+      <c r="ML2" s="50"/>
+      <c r="MM2" s="50"/>
+      <c r="MN2" s="50"/>
+      <c r="MO2" s="50"/>
+      <c r="MP2" s="50"/>
+      <c r="MQ2" s="50"/>
+      <c r="MR2" s="50"/>
+      <c r="MS2" s="50"/>
+      <c r="MT2" s="50"/>
+      <c r="MU2" s="50"/>
+      <c r="MV2" s="50"/>
+      <c r="MW2" s="50"/>
+      <c r="MX2" s="50"/>
+      <c r="MY2" s="50"/>
+      <c r="MZ2" s="50"/>
+      <c r="NA2" s="50"/>
+      <c r="NB2" s="50"/>
+      <c r="NC2" s="50"/>
+      <c r="ND2" s="50"/>
+      <c r="NE2" s="50"/>
+      <c r="NF2" s="51" t="s">
         <v>586</v>
       </c>
-      <c r="NG2" s="67"/>
-      <c r="NH2" s="67"/>
-      <c r="NI2" s="67"/>
-      <c r="NJ2" s="67"/>
-      <c r="NK2" s="67"/>
-      <c r="NL2" s="67"/>
-      <c r="NM2" s="67"/>
-      <c r="NN2" s="67"/>
-      <c r="NO2" s="67"/>
-      <c r="NP2" s="54" t="s">
+      <c r="NG2" s="51"/>
+      <c r="NH2" s="51"/>
+      <c r="NI2" s="51"/>
+      <c r="NJ2" s="51"/>
+      <c r="NK2" s="51"/>
+      <c r="NL2" s="51"/>
+      <c r="NM2" s="51"/>
+      <c r="NN2" s="51"/>
+      <c r="NO2" s="51"/>
+      <c r="NP2" s="64" t="s">
         <v>587</v>
       </c>
-      <c r="NQ2" s="54"/>
-      <c r="NR2" s="54"/>
-      <c r="NS2" s="54"/>
-      <c r="NT2" s="54"/>
-      <c r="NU2" s="54"/>
-      <c r="NV2" s="54"/>
-      <c r="NW2" s="54"/>
-      <c r="NX2" s="54"/>
-      <c r="NY2" s="54"/>
-      <c r="NZ2" s="54"/>
-      <c r="OA2" s="54"/>
-      <c r="OB2" s="54"/>
-      <c r="OC2" s="54"/>
-      <c r="OD2" s="54"/>
-      <c r="OE2" s="54"/>
-      <c r="OF2" s="54"/>
-      <c r="OG2" s="54"/>
-      <c r="OH2" s="54"/>
-      <c r="OI2" s="54"/>
-      <c r="OJ2" s="54"/>
-      <c r="OK2" s="54"/>
-      <c r="OL2" s="54"/>
-      <c r="OM2" s="54"/>
-      <c r="ON2" s="54"/>
-      <c r="OO2" s="54"/>
-      <c r="OP2" s="54"/>
-      <c r="OQ2" s="54"/>
-      <c r="OR2" s="54"/>
-      <c r="OS2" s="54"/>
-      <c r="OT2" s="54"/>
-      <c r="OU2" s="54"/>
-      <c r="OV2" s="54"/>
-      <c r="OW2" s="54"/>
-      <c r="OX2" s="54"/>
-      <c r="OY2" s="54"/>
-      <c r="OZ2" s="54"/>
-      <c r="PA2" s="54"/>
-      <c r="PB2" s="54"/>
-      <c r="PC2" s="54"/>
-      <c r="PD2" s="54"/>
-      <c r="PE2" s="54"/>
-      <c r="PF2" s="54"/>
-      <c r="PG2" s="54"/>
-      <c r="PH2" s="54"/>
-      <c r="PI2" s="54"/>
-      <c r="PJ2" s="54"/>
-      <c r="PK2" s="54"/>
-      <c r="PL2" s="54"/>
-      <c r="PM2" s="54"/>
-      <c r="PN2" s="54"/>
-      <c r="PO2" s="54"/>
-      <c r="PP2" s="54"/>
-      <c r="PQ2" s="54"/>
-      <c r="PR2" s="54"/>
-      <c r="PS2" s="54"/>
-      <c r="PT2" s="54"/>
-      <c r="PU2" s="54"/>
-      <c r="PV2" s="54"/>
-      <c r="PW2" s="54"/>
-      <c r="PX2" s="54"/>
-      <c r="PY2" s="54"/>
-      <c r="PZ2" s="54"/>
-      <c r="QA2" s="54"/>
-      <c r="QB2" s="54"/>
-      <c r="QC2" s="54"/>
-      <c r="QD2" s="54"/>
-      <c r="QE2" s="54"/>
-      <c r="QF2" s="54"/>
-      <c r="QG2" s="54"/>
-      <c r="QH2" s="54"/>
-      <c r="QI2" s="54"/>
-      <c r="QJ2" s="54"/>
-      <c r="QK2" s="54"/>
-      <c r="QL2" s="54"/>
-      <c r="QM2" s="54"/>
-      <c r="QN2" s="54"/>
-      <c r="QO2" s="54"/>
-      <c r="QP2" s="54"/>
-      <c r="QQ2" s="54"/>
-      <c r="QR2" s="54"/>
-      <c r="QS2" s="54"/>
-      <c r="QT2" s="54"/>
-      <c r="QU2" s="54"/>
-      <c r="QV2" s="54"/>
-      <c r="QW2" s="54"/>
-      <c r="QX2" s="54"/>
-      <c r="QY2" s="54"/>
-      <c r="QZ2" s="54"/>
-      <c r="RA2" s="56" t="s">
+      <c r="NQ2" s="64"/>
+      <c r="NR2" s="64"/>
+      <c r="NS2" s="64"/>
+      <c r="NT2" s="64"/>
+      <c r="NU2" s="64"/>
+      <c r="NV2" s="64"/>
+      <c r="NW2" s="64"/>
+      <c r="NX2" s="64"/>
+      <c r="NY2" s="64"/>
+      <c r="NZ2" s="64"/>
+      <c r="OA2" s="64"/>
+      <c r="OB2" s="64"/>
+      <c r="OC2" s="64"/>
+      <c r="OD2" s="64"/>
+      <c r="OE2" s="64"/>
+      <c r="OF2" s="64"/>
+      <c r="OG2" s="64"/>
+      <c r="OH2" s="64"/>
+      <c r="OI2" s="64"/>
+      <c r="OJ2" s="64"/>
+      <c r="OK2" s="64"/>
+      <c r="OL2" s="64"/>
+      <c r="OM2" s="64"/>
+      <c r="ON2" s="64"/>
+      <c r="OO2" s="64"/>
+      <c r="OP2" s="64"/>
+      <c r="OQ2" s="64"/>
+      <c r="OR2" s="64"/>
+      <c r="OS2" s="64"/>
+      <c r="OT2" s="64"/>
+      <c r="OU2" s="64"/>
+      <c r="OV2" s="64"/>
+      <c r="OW2" s="64"/>
+      <c r="OX2" s="64"/>
+      <c r="OY2" s="64"/>
+      <c r="OZ2" s="64"/>
+      <c r="PA2" s="64"/>
+      <c r="PB2" s="64"/>
+      <c r="PC2" s="64"/>
+      <c r="PD2" s="64"/>
+      <c r="PE2" s="64"/>
+      <c r="PF2" s="64"/>
+      <c r="PG2" s="64"/>
+      <c r="PH2" s="64"/>
+      <c r="PI2" s="64"/>
+      <c r="PJ2" s="64"/>
+      <c r="PK2" s="64"/>
+      <c r="PL2" s="64"/>
+      <c r="PM2" s="64"/>
+      <c r="PN2" s="64"/>
+      <c r="PO2" s="64"/>
+      <c r="PP2" s="64"/>
+      <c r="PQ2" s="64"/>
+      <c r="PR2" s="64"/>
+      <c r="PS2" s="64"/>
+      <c r="PT2" s="64"/>
+      <c r="PU2" s="64"/>
+      <c r="PV2" s="64"/>
+      <c r="PW2" s="64"/>
+      <c r="PX2" s="64"/>
+      <c r="PY2" s="64"/>
+      <c r="PZ2" s="64"/>
+      <c r="QA2" s="64"/>
+      <c r="QB2" s="64"/>
+      <c r="QC2" s="64"/>
+      <c r="QD2" s="64"/>
+      <c r="QE2" s="64"/>
+      <c r="QF2" s="64"/>
+      <c r="QG2" s="64"/>
+      <c r="QH2" s="64"/>
+      <c r="QI2" s="64"/>
+      <c r="QJ2" s="64"/>
+      <c r="QK2" s="64"/>
+      <c r="QL2" s="64"/>
+      <c r="QM2" s="64"/>
+      <c r="QN2" s="64"/>
+      <c r="QO2" s="64"/>
+      <c r="QP2" s="64"/>
+      <c r="QQ2" s="64"/>
+      <c r="QR2" s="64"/>
+      <c r="QS2" s="64"/>
+      <c r="QT2" s="64"/>
+      <c r="QU2" s="64"/>
+      <c r="QV2" s="64"/>
+      <c r="QW2" s="64"/>
+      <c r="QX2" s="64"/>
+      <c r="QY2" s="64"/>
+      <c r="QZ2" s="64"/>
+      <c r="RA2" s="66" t="s">
         <v>592</v>
       </c>
-      <c r="RB2" s="56"/>
-      <c r="RC2" s="56"/>
-      <c r="RD2" s="56"/>
-      <c r="RE2" s="56"/>
-      <c r="RF2" s="56"/>
-      <c r="RG2" s="56"/>
-      <c r="RH2" s="56"/>
-      <c r="RI2" s="56"/>
-      <c r="RJ2" s="56"/>
-      <c r="RK2" s="56"/>
-      <c r="RL2" s="56"/>
-      <c r="RM2" s="56"/>
-      <c r="RN2" s="56"/>
-      <c r="RO2" s="56"/>
-      <c r="RP2" s="56"/>
-      <c r="RQ2" s="56"/>
-      <c r="RR2" s="56"/>
-      <c r="RS2" s="56"/>
-      <c r="RT2" s="56"/>
-      <c r="RU2" s="56"/>
-      <c r="RV2" s="56"/>
-      <c r="RW2" s="56"/>
-      <c r="RX2" s="56"/>
-      <c r="RY2" s="56"/>
-      <c r="RZ2" s="56"/>
-      <c r="SA2" s="56"/>
-      <c r="SB2" s="56"/>
-      <c r="SC2" s="56"/>
-      <c r="SD2" s="56"/>
-      <c r="SE2" s="56"/>
-      <c r="SF2" s="56"/>
-      <c r="SG2" s="56"/>
-      <c r="SH2" s="56"/>
-      <c r="SI2" s="56"/>
-      <c r="SJ2" s="56"/>
-      <c r="SK2" s="56"/>
-      <c r="SL2" s="56"/>
-      <c r="SM2" s="56"/>
-      <c r="SN2" s="56"/>
-      <c r="SO2" s="56"/>
-      <c r="SP2" s="56"/>
-      <c r="SQ2" s="56"/>
-      <c r="SR2" s="56"/>
-      <c r="SS2" s="56"/>
-      <c r="ST2" s="56"/>
-      <c r="SU2" s="56"/>
-      <c r="SV2" s="56"/>
-      <c r="SW2" s="56"/>
-      <c r="SX2" s="56"/>
-      <c r="SY2" s="56"/>
-      <c r="SZ2" s="56"/>
-      <c r="TA2" s="56"/>
-      <c r="TB2" s="56"/>
-      <c r="TC2" s="56"/>
-      <c r="TD2" s="56"/>
-      <c r="TE2" s="56"/>
-      <c r="TF2" s="56"/>
-      <c r="TG2" s="56"/>
-      <c r="TH2" s="56"/>
-      <c r="TI2" s="53" t="s">
+      <c r="RB2" s="66"/>
+      <c r="RC2" s="66"/>
+      <c r="RD2" s="66"/>
+      <c r="RE2" s="66"/>
+      <c r="RF2" s="66"/>
+      <c r="RG2" s="66"/>
+      <c r="RH2" s="66"/>
+      <c r="RI2" s="66"/>
+      <c r="RJ2" s="66"/>
+      <c r="RK2" s="66"/>
+      <c r="RL2" s="66"/>
+      <c r="RM2" s="66"/>
+      <c r="RN2" s="66"/>
+      <c r="RO2" s="66"/>
+      <c r="RP2" s="66"/>
+      <c r="RQ2" s="66"/>
+      <c r="RR2" s="66"/>
+      <c r="RS2" s="66"/>
+      <c r="RT2" s="66"/>
+      <c r="RU2" s="66"/>
+      <c r="RV2" s="66"/>
+      <c r="RW2" s="66"/>
+      <c r="RX2" s="66"/>
+      <c r="RY2" s="66"/>
+      <c r="RZ2" s="66"/>
+      <c r="SA2" s="66"/>
+      <c r="SB2" s="66"/>
+      <c r="SC2" s="66"/>
+      <c r="SD2" s="66"/>
+      <c r="SE2" s="66"/>
+      <c r="SF2" s="66"/>
+      <c r="SG2" s="66"/>
+      <c r="SH2" s="66"/>
+      <c r="SI2" s="66"/>
+      <c r="SJ2" s="66"/>
+      <c r="SK2" s="66"/>
+      <c r="SL2" s="66"/>
+      <c r="SM2" s="66"/>
+      <c r="SN2" s="66"/>
+      <c r="SO2" s="66"/>
+      <c r="SP2" s="66"/>
+      <c r="SQ2" s="66"/>
+      <c r="SR2" s="66"/>
+      <c r="SS2" s="66"/>
+      <c r="ST2" s="66"/>
+      <c r="SU2" s="66"/>
+      <c r="SV2" s="66"/>
+      <c r="SW2" s="66"/>
+      <c r="SX2" s="66"/>
+      <c r="SY2" s="66"/>
+      <c r="SZ2" s="66"/>
+      <c r="TA2" s="66"/>
+      <c r="TB2" s="66"/>
+      <c r="TC2" s="66"/>
+      <c r="TD2" s="66"/>
+      <c r="TE2" s="66"/>
+      <c r="TF2" s="66"/>
+      <c r="TG2" s="66"/>
+      <c r="TH2" s="66"/>
+      <c r="TI2" s="55" t="s">
         <v>593</v>
       </c>
-      <c r="TJ2" s="53"/>
-      <c r="TK2" s="53"/>
-      <c r="TL2" s="53"/>
-      <c r="TM2" s="53"/>
-      <c r="TN2" s="53"/>
-      <c r="TO2" s="68" t="s">
+      <c r="TJ2" s="55"/>
+      <c r="TK2" s="55"/>
+      <c r="TL2" s="55"/>
+      <c r="TM2" s="55"/>
+      <c r="TN2" s="55"/>
+      <c r="TO2" s="56" t="s">
         <v>594</v>
       </c>
-      <c r="TP2" s="68"/>
-      <c r="TQ2" s="68"/>
-      <c r="TR2" s="68"/>
-      <c r="TS2" s="68"/>
-      <c r="TT2" s="68"/>
-      <c r="TU2" s="68"/>
-      <c r="TV2" s="68"/>
-      <c r="TW2" s="68"/>
-      <c r="TX2" s="68"/>
-      <c r="TY2" s="68"/>
-      <c r="TZ2" s="68"/>
-      <c r="UA2" s="68"/>
-      <c r="UB2" s="68"/>
-      <c r="UC2" s="68"/>
-      <c r="UD2" s="68"/>
-      <c r="UE2" s="68"/>
-      <c r="UF2" s="68"/>
-      <c r="UG2" s="68"/>
-      <c r="UH2" s="68"/>
-      <c r="UI2" s="68"/>
-      <c r="UJ2" s="68"/>
-      <c r="UK2" s="68"/>
-      <c r="UL2" s="68"/>
-      <c r="UM2" s="68"/>
-      <c r="UN2" s="68"/>
-      <c r="UO2" s="68"/>
-      <c r="UP2" s="68"/>
-      <c r="UQ2" s="68"/>
-      <c r="UR2" s="68"/>
-      <c r="US2" s="68"/>
-      <c r="UT2" s="68"/>
-      <c r="UU2" s="68"/>
-      <c r="UV2" s="68"/>
-      <c r="UW2" s="68"/>
-      <c r="UX2" s="68"/>
-      <c r="UY2" s="68"/>
-      <c r="UZ2" s="68"/>
-      <c r="VA2" s="68"/>
-      <c r="VB2" s="68"/>
-      <c r="VC2" s="68"/>
-      <c r="VD2" s="68"/>
-      <c r="VE2" s="68"/>
-      <c r="VF2" s="68"/>
-      <c r="VG2" s="68"/>
-      <c r="VH2" s="68"/>
-      <c r="VI2" s="68"/>
-      <c r="VJ2" s="68"/>
-      <c r="VK2" s="68"/>
-      <c r="VL2" s="68"/>
-      <c r="VM2" s="68"/>
-      <c r="VN2" s="68"/>
-      <c r="VO2" s="68"/>
-      <c r="VP2" s="68"/>
-      <c r="VQ2" s="68"/>
-      <c r="VR2" s="68"/>
-      <c r="VS2" s="68"/>
-      <c r="VT2" s="68"/>
-      <c r="VU2" s="68"/>
-      <c r="VV2" s="68"/>
-      <c r="VW2" s="68"/>
-      <c r="VX2" s="68"/>
-      <c r="VY2" s="68"/>
-      <c r="VZ2" s="68"/>
-      <c r="WA2" s="68"/>
-      <c r="WB2" s="68"/>
-      <c r="WC2" s="68"/>
-      <c r="WD2" s="68"/>
-      <c r="WE2" s="68"/>
-      <c r="WF2" s="68"/>
-      <c r="WG2" s="68"/>
-      <c r="WH2" s="68"/>
-      <c r="WI2" s="68"/>
-      <c r="WJ2" s="68"/>
-      <c r="WK2" s="68"/>
-      <c r="WL2" s="68"/>
-      <c r="WM2" s="68"/>
-      <c r="WN2" s="68"/>
-      <c r="WO2" s="68"/>
-      <c r="WP2" s="68"/>
-      <c r="WQ2" s="68"/>
-      <c r="WR2" s="68"/>
-      <c r="WS2" s="68"/>
-      <c r="WT2" s="68"/>
-      <c r="WU2" s="62" t="s">
+      <c r="TP2" s="56"/>
+      <c r="TQ2" s="56"/>
+      <c r="TR2" s="56"/>
+      <c r="TS2" s="56"/>
+      <c r="TT2" s="56"/>
+      <c r="TU2" s="56"/>
+      <c r="TV2" s="56"/>
+      <c r="TW2" s="56"/>
+      <c r="TX2" s="56"/>
+      <c r="TY2" s="56"/>
+      <c r="TZ2" s="56"/>
+      <c r="UA2" s="56"/>
+      <c r="UB2" s="56"/>
+      <c r="UC2" s="56"/>
+      <c r="UD2" s="56"/>
+      <c r="UE2" s="56"/>
+      <c r="UF2" s="56"/>
+      <c r="UG2" s="56"/>
+      <c r="UH2" s="56"/>
+      <c r="UI2" s="56"/>
+      <c r="UJ2" s="56"/>
+      <c r="UK2" s="56"/>
+      <c r="UL2" s="56"/>
+      <c r="UM2" s="56"/>
+      <c r="UN2" s="56"/>
+      <c r="UO2" s="56"/>
+      <c r="UP2" s="56"/>
+      <c r="UQ2" s="56"/>
+      <c r="UR2" s="56"/>
+      <c r="US2" s="56"/>
+      <c r="UT2" s="56"/>
+      <c r="UU2" s="56"/>
+      <c r="UV2" s="56"/>
+      <c r="UW2" s="56"/>
+      <c r="UX2" s="56"/>
+      <c r="UY2" s="56"/>
+      <c r="UZ2" s="56"/>
+      <c r="VA2" s="56"/>
+      <c r="VB2" s="56"/>
+      <c r="VC2" s="56"/>
+      <c r="VD2" s="56"/>
+      <c r="VE2" s="56"/>
+      <c r="VF2" s="56"/>
+      <c r="VG2" s="56"/>
+      <c r="VH2" s="56"/>
+      <c r="VI2" s="56"/>
+      <c r="VJ2" s="56"/>
+      <c r="VK2" s="56"/>
+      <c r="VL2" s="56"/>
+      <c r="VM2" s="56"/>
+      <c r="VN2" s="56"/>
+      <c r="VO2" s="56"/>
+      <c r="VP2" s="56"/>
+      <c r="VQ2" s="56"/>
+      <c r="VR2" s="56"/>
+      <c r="VS2" s="56"/>
+      <c r="VT2" s="56"/>
+      <c r="VU2" s="56"/>
+      <c r="VV2" s="56"/>
+      <c r="VW2" s="56"/>
+      <c r="VX2" s="56"/>
+      <c r="VY2" s="56"/>
+      <c r="VZ2" s="56"/>
+      <c r="WA2" s="56"/>
+      <c r="WB2" s="56"/>
+      <c r="WC2" s="56"/>
+      <c r="WD2" s="56"/>
+      <c r="WE2" s="56"/>
+      <c r="WF2" s="56"/>
+      <c r="WG2" s="56"/>
+      <c r="WH2" s="56"/>
+      <c r="WI2" s="56"/>
+      <c r="WJ2" s="56"/>
+      <c r="WK2" s="56"/>
+      <c r="WL2" s="56"/>
+      <c r="WM2" s="56"/>
+      <c r="WN2" s="56"/>
+      <c r="WO2" s="56"/>
+      <c r="WP2" s="56"/>
+      <c r="WQ2" s="56"/>
+      <c r="WR2" s="56"/>
+      <c r="WS2" s="56"/>
+      <c r="WT2" s="56"/>
+      <c r="WU2" s="54" t="s">
         <v>603</v>
       </c>
-      <c r="WV2" s="62"/>
-      <c r="WW2" s="62"/>
-      <c r="WX2" s="62"/>
-      <c r="WY2" s="62"/>
-      <c r="WZ2" s="62"/>
-      <c r="XA2" s="62"/>
-      <c r="XB2" s="62"/>
-      <c r="XC2" s="62"/>
-      <c r="XD2" s="62"/>
-      <c r="XE2" s="62"/>
-      <c r="XF2" s="62"/>
-      <c r="XG2" s="62"/>
-      <c r="XH2" s="62"/>
-      <c r="XI2" s="62"/>
-      <c r="XJ2" s="62"/>
-      <c r="XK2" s="62"/>
-      <c r="XL2" s="62"/>
-      <c r="XM2" s="62"/>
-      <c r="XN2" s="62"/>
-      <c r="XO2" s="62"/>
-      <c r="XP2" s="62"/>
-      <c r="XQ2" s="62"/>
-      <c r="XR2" s="62"/>
-      <c r="XS2" s="58" t="s">
+      <c r="WV2" s="54"/>
+      <c r="WW2" s="54"/>
+      <c r="WX2" s="54"/>
+      <c r="WY2" s="54"/>
+      <c r="WZ2" s="54"/>
+      <c r="XA2" s="54"/>
+      <c r="XB2" s="54"/>
+      <c r="XC2" s="54"/>
+      <c r="XD2" s="54"/>
+      <c r="XE2" s="54"/>
+      <c r="XF2" s="54"/>
+      <c r="XG2" s="54"/>
+      <c r="XH2" s="54"/>
+      <c r="XI2" s="54"/>
+      <c r="XJ2" s="54"/>
+      <c r="XK2" s="54"/>
+      <c r="XL2" s="54"/>
+      <c r="XM2" s="54"/>
+      <c r="XN2" s="54"/>
+      <c r="XO2" s="54"/>
+      <c r="XP2" s="54"/>
+      <c r="XQ2" s="54"/>
+      <c r="XR2" s="54"/>
+      <c r="XS2" s="53" t="s">
         <v>607</v>
       </c>
-      <c r="XT2" s="58"/>
-      <c r="XU2" s="58"/>
-      <c r="XV2" s="58"/>
-      <c r="XW2" s="58"/>
-      <c r="XX2" s="58"/>
-      <c r="XY2" s="58"/>
-      <c r="XZ2" s="58"/>
-      <c r="YA2" s="58"/>
-      <c r="YB2" s="58"/>
-      <c r="YC2" s="58"/>
-      <c r="YD2" s="58"/>
-      <c r="YE2" s="58"/>
-      <c r="YF2" s="58"/>
-      <c r="YG2" s="58"/>
-      <c r="YH2" s="58"/>
-      <c r="YI2" s="58"/>
-      <c r="YJ2" s="58"/>
-      <c r="YK2" s="58"/>
-      <c r="YL2" s="58"/>
-      <c r="YM2" s="58"/>
-      <c r="YN2" s="58"/>
-      <c r="YO2" s="58"/>
-      <c r="YP2" s="58"/>
-      <c r="YQ2" s="58"/>
-      <c r="YR2" s="58"/>
-      <c r="YS2" s="58"/>
-      <c r="YT2" s="58"/>
-      <c r="YU2" s="58"/>
-      <c r="YV2" s="58"/>
-      <c r="YW2" s="58"/>
-      <c r="YX2" s="58"/>
-      <c r="YY2" s="58"/>
-      <c r="YZ2" s="58"/>
-      <c r="ZA2" s="58"/>
-      <c r="ZB2" s="58"/>
-      <c r="ZC2" s="58"/>
-      <c r="ZD2" s="58"/>
-      <c r="ZE2" s="58"/>
-      <c r="ZF2" s="58"/>
-      <c r="ZG2" s="58"/>
-      <c r="ZH2" s="58"/>
-      <c r="ZI2" s="58"/>
-      <c r="ZJ2" s="58"/>
-      <c r="ZK2" s="58"/>
-      <c r="ZL2" s="60" t="s">
+      <c r="XT2" s="53"/>
+      <c r="XU2" s="53"/>
+      <c r="XV2" s="53"/>
+      <c r="XW2" s="53"/>
+      <c r="XX2" s="53"/>
+      <c r="XY2" s="53"/>
+      <c r="XZ2" s="53"/>
+      <c r="YA2" s="53"/>
+      <c r="YB2" s="53"/>
+      <c r="YC2" s="53"/>
+      <c r="YD2" s="53"/>
+      <c r="YE2" s="53"/>
+      <c r="YF2" s="53"/>
+      <c r="YG2" s="53"/>
+      <c r="YH2" s="53"/>
+      <c r="YI2" s="53"/>
+      <c r="YJ2" s="53"/>
+      <c r="YK2" s="53"/>
+      <c r="YL2" s="53"/>
+      <c r="YM2" s="53"/>
+      <c r="YN2" s="53"/>
+      <c r="YO2" s="53"/>
+      <c r="YP2" s="53"/>
+      <c r="YQ2" s="53"/>
+      <c r="YR2" s="53"/>
+      <c r="YS2" s="53"/>
+      <c r="YT2" s="53"/>
+      <c r="YU2" s="53"/>
+      <c r="YV2" s="53"/>
+      <c r="YW2" s="53"/>
+      <c r="YX2" s="53"/>
+      <c r="YY2" s="53"/>
+      <c r="YZ2" s="53"/>
+      <c r="ZA2" s="53"/>
+      <c r="ZB2" s="53"/>
+      <c r="ZC2" s="53"/>
+      <c r="ZD2" s="53"/>
+      <c r="ZE2" s="53"/>
+      <c r="ZF2" s="53"/>
+      <c r="ZG2" s="53"/>
+      <c r="ZH2" s="53"/>
+      <c r="ZI2" s="53"/>
+      <c r="ZJ2" s="53"/>
+      <c r="ZK2" s="53"/>
+      <c r="ZL2" s="52" t="s">
         <v>608</v>
       </c>
-      <c r="ZM2" s="60"/>
-      <c r="ZN2" s="60"/>
-      <c r="ZO2" s="60"/>
-      <c r="ZP2" s="60"/>
-      <c r="ZQ2" s="60"/>
-      <c r="ZR2" s="60"/>
-      <c r="ZS2" s="60"/>
-      <c r="ZT2" s="60"/>
-      <c r="ZU2" s="60"/>
-      <c r="ZV2" s="60"/>
-      <c r="ZW2" s="60"/>
+      <c r="ZM2" s="52"/>
+      <c r="ZN2" s="52"/>
+      <c r="ZO2" s="52"/>
+      <c r="ZP2" s="52"/>
+      <c r="ZQ2" s="52"/>
+      <c r="ZR2" s="52"/>
+      <c r="ZS2" s="52"/>
+      <c r="ZT2" s="52"/>
+      <c r="ZU2" s="52"/>
+      <c r="ZV2" s="52"/>
+      <c r="ZW2" s="52"/>
       <c r="ZX2" s="47" t="s">
         <v>1176</v>
       </c>
@@ -19000,7 +19081,7 @@
       <c r="ADE2" s="49"/>
     </row>
     <row r="3" spans="1:785 16376:16376" s="25" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="52"/>
+      <c r="A3" s="63"/>
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -20120,13 +20201,13 @@
       <c r="NJ3" s="15" t="s">
         <v>732</v>
       </c>
-      <c r="NK3" s="50" t="s">
+      <c r="NK3" s="61" t="s">
         <v>733</v>
       </c>
-      <c r="NL3" s="50"/>
-      <c r="NM3" s="50"/>
-      <c r="NN3" s="50"/>
-      <c r="NO3" s="50"/>
+      <c r="NL3" s="61"/>
+      <c r="NM3" s="61"/>
+      <c r="NN3" s="61"/>
+      <c r="NO3" s="61"/>
       <c r="NP3" s="16" t="s">
         <v>734</v>
       </c>
@@ -40832,25 +40913,6 @@
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="ABB2:ABK2"/>
-    <mergeCell ref="ABL2:ABU2"/>
-    <mergeCell ref="ABV2:ACE2"/>
-    <mergeCell ref="ZX2:AAC2"/>
-    <mergeCell ref="AAD2:AAI2"/>
-    <mergeCell ref="AAS2:AAX2"/>
-    <mergeCell ref="AAJ2:AAR2"/>
-    <mergeCell ref="JT2:NE2"/>
-    <mergeCell ref="NF2:NO2"/>
-    <mergeCell ref="ZL2:ZW2"/>
-    <mergeCell ref="XS2:ZK2"/>
-    <mergeCell ref="WU2:XR2"/>
-    <mergeCell ref="TI2:TN2"/>
-    <mergeCell ref="TO2:WT2"/>
-    <mergeCell ref="DY2:FA2"/>
-    <mergeCell ref="FB2:FE2"/>
-    <mergeCell ref="FF2:GA2"/>
-    <mergeCell ref="GB2:GL2"/>
-    <mergeCell ref="GM2:HO2"/>
     <mergeCell ref="ACV2:ADE2"/>
     <mergeCell ref="ACF2:ACK2"/>
     <mergeCell ref="ACO2:ACT2"/>
@@ -40867,6 +40929,25 @@
     <mergeCell ref="HP2:IC2"/>
     <mergeCell ref="ID2:IO2"/>
     <mergeCell ref="IP2:JS2"/>
+    <mergeCell ref="DY2:FA2"/>
+    <mergeCell ref="FB2:FE2"/>
+    <mergeCell ref="FF2:GA2"/>
+    <mergeCell ref="GB2:GL2"/>
+    <mergeCell ref="GM2:HO2"/>
+    <mergeCell ref="JT2:NE2"/>
+    <mergeCell ref="NF2:NO2"/>
+    <mergeCell ref="ZL2:ZW2"/>
+    <mergeCell ref="XS2:ZK2"/>
+    <mergeCell ref="WU2:XR2"/>
+    <mergeCell ref="TI2:TN2"/>
+    <mergeCell ref="TO2:WT2"/>
+    <mergeCell ref="ABB2:ABK2"/>
+    <mergeCell ref="ABL2:ABU2"/>
+    <mergeCell ref="ABV2:ACE2"/>
+    <mergeCell ref="ZX2:AAC2"/>
+    <mergeCell ref="AAD2:AAI2"/>
+    <mergeCell ref="AAS2:AAX2"/>
+    <mergeCell ref="AAJ2:AAR2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -40888,122 +40969,122 @@
   <sheetData>
     <row r="4" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C4" t="s">
-        <v>1890</v>
+        <v>1885</v>
       </c>
     </row>
     <row r="5" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C5" t="s">
-        <v>1891</v>
+        <v>1886</v>
       </c>
     </row>
     <row r="6" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C6" t="s">
-        <v>1892</v>
+        <v>1887</v>
       </c>
     </row>
     <row r="7" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C7" t="s">
-        <v>1893</v>
+        <v>1888</v>
       </c>
     </row>
     <row r="8" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C8" t="s">
-        <v>1894</v>
+        <v>1889</v>
       </c>
     </row>
     <row r="9" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C9" t="s">
-        <v>1895</v>
+        <v>1890</v>
       </c>
     </row>
     <row r="10" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C10" t="s">
-        <v>1896</v>
+        <v>1891</v>
       </c>
     </row>
     <row r="11" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C11" t="s">
-        <v>1897</v>
+        <v>1892</v>
       </c>
     </row>
     <row r="12" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C12" t="s">
-        <v>1898</v>
+        <v>1893</v>
       </c>
     </row>
     <row r="13" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C13" t="s">
-        <v>1899</v>
+        <v>1894</v>
       </c>
     </row>
     <row r="14" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C14" t="s">
-        <v>1900</v>
+        <v>1895</v>
       </c>
     </row>
     <row r="15" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C15" t="s">
-        <v>1901</v>
+        <v>1896</v>
       </c>
     </row>
     <row r="16" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C16" t="s">
-        <v>1902</v>
+        <v>1897</v>
       </c>
     </row>
     <row r="17" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C17" t="s">
-        <v>1903</v>
+        <v>1898</v>
       </c>
     </row>
     <row r="18" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C18" t="s">
-        <v>1904</v>
+        <v>1899</v>
       </c>
     </row>
     <row r="19" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C19" t="s">
-        <v>1905</v>
+        <v>1900</v>
       </c>
     </row>
     <row r="20" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C20" t="s">
-        <v>1906</v>
+        <v>1901</v>
       </c>
     </row>
     <row r="21" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C21" t="s">
-        <v>1907</v>
+        <v>1902</v>
       </c>
     </row>
     <row r="22" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C22" t="s">
-        <v>1908</v>
+        <v>1903</v>
       </c>
     </row>
     <row r="23" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C23" t="s">
-        <v>1909</v>
+        <v>1904</v>
       </c>
     </row>
     <row r="24" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C24" t="s">
-        <v>1910</v>
+        <v>1905</v>
       </c>
     </row>
     <row r="25" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C25" t="s">
-        <v>1911</v>
+        <v>1906</v>
       </c>
     </row>
     <row r="26" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C26" t="s">
-        <v>1912</v>
+        <v>1907</v>
       </c>
     </row>
     <row r="27" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C27" t="s">
-        <v>1913</v>
+        <v>1908</v>
       </c>
     </row>
     <row r="28" spans="3:3" x14ac:dyDescent="0.35">
@@ -41013,47 +41094,47 @@
     </row>
     <row r="29" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C29" t="s">
-        <v>1914</v>
+        <v>1909</v>
       </c>
     </row>
     <row r="30" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C30" t="s">
-        <v>1915</v>
+        <v>1910</v>
       </c>
     </row>
     <row r="31" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C31" t="s">
-        <v>1916</v>
+        <v>1911</v>
       </c>
     </row>
     <row r="32" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C32" t="s">
-        <v>1917</v>
+        <v>1912</v>
       </c>
     </row>
     <row r="33" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C33" t="s">
-        <v>1918</v>
+        <v>1913</v>
       </c>
     </row>
     <row r="34" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C34" t="s">
-        <v>1919</v>
+        <v>1914</v>
       </c>
     </row>
     <row r="35" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C35" t="s">
-        <v>1920</v>
+        <v>1915</v>
       </c>
     </row>
     <row r="36" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C36" t="s">
-        <v>1921</v>
+        <v>1916</v>
       </c>
     </row>
     <row r="37" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C37" t="s">
-        <v>1922</v>
+        <v>1917</v>
       </c>
     </row>
     <row r="38" spans="3:3" x14ac:dyDescent="0.35">
@@ -41063,27 +41144,27 @@
     </row>
     <row r="39" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C39" t="s">
-        <v>1923</v>
+        <v>1918</v>
       </c>
     </row>
     <row r="40" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C40" t="s">
-        <v>1924</v>
+        <v>1919</v>
       </c>
     </row>
     <row r="41" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C41" t="s">
-        <v>1925</v>
+        <v>1920</v>
       </c>
     </row>
     <row r="42" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C42" t="s">
-        <v>1926</v>
+        <v>1921</v>
       </c>
     </row>
     <row r="43" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C43" t="s">
-        <v>1927</v>
+        <v>1922</v>
       </c>
     </row>
   </sheetData>
@@ -41122,14 +41203,14 @@
       <c r="N1" s="83"/>
       <c r="O1" s="83"/>
       <c r="P1" s="83"/>
-      <c r="Q1" s="54" t="s">
+      <c r="Q1" s="64" t="s">
         <v>177</v>
       </c>
-      <c r="R1" s="54"/>
-      <c r="S1" s="54"/>
-      <c r="T1" s="54"/>
-      <c r="U1" s="54"/>
-      <c r="V1" s="54"/>
+      <c r="R1" s="64"/>
+      <c r="S1" s="64"/>
+      <c r="T1" s="64"/>
+      <c r="U1" s="64"/>
+      <c r="V1" s="64"/>
       <c r="W1" s="84" t="s">
         <v>262</v>
       </c>

</xml_diff>